<commit_message>
aggiornamento dati 01/03 e rigen. report
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1896,8 +1896,12 @@
       <c r="B110" t="n">
         <v>3</v>
       </c>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="C110" t="n">
+        <v>12</v>
+      </c>
+      <c r="D110" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -1918,6 +1922,16 @@
       </c>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B113" t="n">
+        <v>5</v>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
aggiornato a 2/3, aggiornati i report
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1617,10 +1617,10 @@
         <v>1</v>
       </c>
       <c r="C90" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D90" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="91">
@@ -1631,10 +1631,10 @@
         <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D91" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="92">
@@ -1645,57 +1645,57 @@
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D92" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44236</v>
+        <v>44235</v>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C93" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D93" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44237</v>
+        <v>44236</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D94" t="n">
-        <v>23.82654276864427</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44238</v>
+        <v>44237</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44239</v>
+        <v>44238</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
@@ -1709,21 +1709,21 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44240</v>
+        <v>44239</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44241</v>
+        <v>44240</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44242</v>
+        <v>44241</v>
       </c>
       <c r="B99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
         <v>3</v>
@@ -1751,63 +1751,63 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44243</v>
+        <v>44242</v>
       </c>
       <c r="B100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C100" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D100" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44244</v>
+        <v>44243</v>
       </c>
       <c r="B101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D101" t="n">
-        <v>166.7857993805099</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="B102" t="n">
         <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D102" t="n">
-        <v>262.091970455087</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44246</v>
+        <v>44245</v>
       </c>
       <c r="B103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D103" t="n">
-        <v>238.2654276864427</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44247</v>
+        <v>44246</v>
       </c>
       <c r="B104" t="n">
         <v>2</v>
@@ -1821,10 +1821,10 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44248</v>
+        <v>44247</v>
       </c>
       <c r="B105" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C105" t="n">
         <v>10</v>
@@ -1835,103 +1835,131 @@
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44249</v>
+        <v>44248</v>
       </c>
       <c r="B106" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C106" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D106" t="n">
-        <v>262.091970455087</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44250</v>
+        <v>44249</v>
       </c>
       <c r="B107" t="n">
         <v>1</v>
       </c>
       <c r="C107" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D107" t="n">
-        <v>285.9185132237312</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44251</v>
+        <v>44250</v>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D108" t="n">
-        <v>238.2654276864427</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44252</v>
+        <v>44251</v>
       </c>
       <c r="B109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D109" t="n">
-        <v>190.6123421491542</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44253</v>
+        <v>44252</v>
       </c>
       <c r="B110" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C110" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D110" t="n">
-        <v>285.9185132237312</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44254</v>
+        <v>44253</v>
       </c>
       <c r="B111" t="n">
-        <v>0</v>
-      </c>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="C111" t="n">
+        <v>12</v>
+      </c>
+      <c r="D111" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44255</v>
+        <v>44254</v>
       </c>
       <c r="B112" t="n">
-        <v>2</v>
-      </c>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C112" t="n">
+        <v>12</v>
+      </c>
+      <c r="D112" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44256</v>
+        <v>44255</v>
       </c>
       <c r="B113" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B114" t="n">
+        <v>5</v>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B115" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
aggiornate un po' di date mancanti da immagini, aggiornati report
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44107</v>
+        <v>44102</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44108</v>
+        <v>44107</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44110</v>
+        <v>44108</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44111</v>
+        <v>44109</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -547,360 +547,360 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44115</v>
+        <v>44110</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44116</v>
+        <v>44111</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44118</v>
+        <v>44113</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44119</v>
+        <v>44114</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44120</v>
+        <v>44115</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>47.65308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44121</v>
+        <v>44116</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>166.7857993805099</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44130</v>
+        <v>44118</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>333.5715987610197</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44137</v>
+        <v>44119</v>
       </c>
       <c r="B21" t="n">
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>333.5715987610197</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44144</v>
+        <v>44120</v>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>381.2246842983083</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44145</v>
+        <v>44121</v>
       </c>
       <c r="B23" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>524.183940910174</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44151</v>
+        <v>44130</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D24" t="n">
-        <v>524.183940910174</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44152</v>
+        <v>44137</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D25" t="n">
-        <v>571.8370264474624</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44153</v>
+        <v>44139</v>
       </c>
       <c r="B26" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D26" t="n">
-        <v>548.0104836788182</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44154</v>
+        <v>44144</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" t="n">
-        <v>452.7043126042411</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44155</v>
+        <v>44145</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C28" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D28" t="n">
-        <v>476.5308553728854</v>
+        <v>619.490111984751</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44156</v>
+        <v>44151</v>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D29" t="n">
-        <v>524.183940910174</v>
+        <v>595.6635692161067</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44157</v>
+        <v>44152</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D30" t="n">
-        <v>428.8777698355968</v>
+        <v>571.8370264474624</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44158</v>
+        <v>44153</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C31" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D31" t="n">
-        <v>500.3573981415297</v>
+        <v>548.0104836788182</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44159</v>
+        <v>44154</v>
       </c>
       <c r="B32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" t="n">
-        <v>476.5308553728854</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44160</v>
+        <v>44155</v>
       </c>
       <c r="B33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D33" t="n">
-        <v>405.0512270669526</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44162</v>
+        <v>44156</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D34" t="n">
-        <v>357.398141529664</v>
+        <v>524.183940910174</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44163</v>
+        <v>44157</v>
       </c>
       <c r="B35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D35" t="n">
-        <v>333.5715987610197</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44164</v>
+        <v>44158</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D36" t="n">
-        <v>238.2654276864427</v>
+        <v>500.3573981415297</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44165</v>
+        <v>44159</v>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D37" t="n">
-        <v>333.5715987610197</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44166</v>
+        <v>44160</v>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D38" t="n">
-        <v>357.398141529664</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44167</v>
+        <v>44162</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C39" t="n">
         <v>15</v>
@@ -911,430 +911,430 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44170</v>
+        <v>44163</v>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D40" t="n">
-        <v>452.7043126042411</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44172</v>
+        <v>44164</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D41" t="n">
-        <v>548.0104836788182</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44176</v>
+        <v>44165</v>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D42" t="n">
-        <v>595.6635692161067</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44177</v>
+        <v>44166</v>
       </c>
       <c r="B43" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D43" t="n">
-        <v>595.6635692161067</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44178</v>
+        <v>44167</v>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D44" t="n">
-        <v>548.0104836788182</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44180</v>
+        <v>44168</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D45" t="n">
-        <v>500.3573981415297</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44181</v>
+        <v>44169</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D46" t="n">
-        <v>524.183940910174</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44182</v>
+        <v>44170</v>
       </c>
       <c r="B47" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C47" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D47" t="n">
-        <v>405.0512270669526</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44183</v>
+        <v>44172</v>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D48" t="n">
-        <v>285.9185132237312</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44184</v>
+        <v>44173</v>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D49" t="n">
-        <v>214.4388849177984</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44185</v>
+        <v>44174</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D50" t="n">
-        <v>262.091970455087</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44187</v>
+        <v>44175</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D51" t="n">
-        <v>238.2654276864427</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44189</v>
+        <v>44176</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C52" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D52" t="n">
-        <v>190.6123421491542</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44190</v>
+        <v>44177</v>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D53" t="n">
-        <v>214.4388849177984</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44192</v>
+        <v>44178</v>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C54" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D54" t="n">
-        <v>262.091970455087</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44194</v>
+        <v>44179</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D55" t="n">
-        <v>262.091970455087</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>44196</v>
+        <v>44180</v>
       </c>
       <c r="B56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D56" t="n">
-        <v>285.9185132237312</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>44197</v>
+        <v>44181</v>
       </c>
       <c r="B57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D57" t="n">
-        <v>238.2654276864427</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>44198</v>
+        <v>44182</v>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C58" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D58" t="n">
-        <v>214.4388849177984</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>44199</v>
+        <v>44183</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D59" t="n">
-        <v>238.2654276864427</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>44200</v>
+        <v>44184</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D60" t="n">
-        <v>142.9592566118656</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>44201</v>
+        <v>44185</v>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D61" t="n">
-        <v>119.1327138432213</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>44204</v>
+        <v>44187</v>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D62" t="n">
-        <v>142.9592566118656</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>44205</v>
+        <v>44188</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
-        <v>119.1327138432213</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>44206</v>
+        <v>44189</v>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>44207</v>
+        <v>44190</v>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C65" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>44208</v>
+        <v>44192</v>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D66" t="n">
-        <v>142.9592566118656</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>44209</v>
+        <v>44194</v>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D67" t="n">
-        <v>142.9592566118656</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>44210</v>
+        <v>44195</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D68" t="n">
-        <v>142.9592566118656</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44211</v>
+        <v>44196</v>
       </c>
       <c r="B69" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C69" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D69" t="n">
-        <v>142.9592566118656</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44212</v>
+        <v>44197</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C70" t="n">
         <v>8</v>
@@ -1345,77 +1345,77 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>44213</v>
+        <v>44198</v>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D71" t="n">
-        <v>166.7857993805099</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>44214</v>
+        <v>44199</v>
       </c>
       <c r="B72" t="n">
         <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D72" t="n">
-        <v>166.7857993805099</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>44215</v>
+        <v>44200</v>
       </c>
       <c r="B73" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D73" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>44216</v>
+        <v>44201</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>44217</v>
+        <v>44204</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>44218</v>
+        <v>44205</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
@@ -1429,161 +1429,161 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>44219</v>
+        <v>44206</v>
       </c>
       <c r="B77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D77" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>44220</v>
+        <v>44207</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D78" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>44221</v>
+        <v>44208</v>
       </c>
       <c r="B79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>44222</v>
+        <v>44209</v>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D80" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>44223</v>
+        <v>44210</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D81" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>44224</v>
+        <v>44211</v>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C82" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D82" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>44225</v>
+        <v>44212</v>
       </c>
       <c r="B83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D83" t="n">
-        <v>71.47962830593281</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>44226</v>
+        <v>44213</v>
       </c>
       <c r="B84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D84" t="n">
-        <v>95.30617107457708</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>44227</v>
+        <v>44214</v>
       </c>
       <c r="B85" t="n">
         <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D85" t="n">
-        <v>95.30617107457708</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>44228</v>
+        <v>44215</v>
       </c>
       <c r="B86" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D86" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>44229</v>
+        <v>44216</v>
       </c>
       <c r="B87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>44230</v>
+        <v>44217</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
@@ -1597,77 +1597,77 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>44231</v>
+        <v>44218</v>
       </c>
       <c r="B89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D89" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>44232</v>
+        <v>44219</v>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D90" t="n">
-        <v>142.9592566118656</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>44233</v>
+        <v>44220</v>
       </c>
       <c r="B91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D91" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>44234</v>
+        <v>44221</v>
       </c>
       <c r="B92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D92" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44235</v>
+        <v>44222</v>
       </c>
       <c r="B93" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D93" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44236</v>
+        <v>44223</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
@@ -1681,94 +1681,94 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44237</v>
+        <v>44224</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D95" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44238</v>
+        <v>44225</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D96" t="n">
-        <v>47.65308553728854</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44239</v>
+        <v>44226</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D97" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44240</v>
+        <v>44227</v>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D98" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44241</v>
+        <v>44228</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D99" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44242</v>
+        <v>44229</v>
       </c>
       <c r="B100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C100" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D100" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44243</v>
+        <v>44230</v>
       </c>
       <c r="B101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" t="n">
         <v>5</v>
@@ -1779,187 +1779,369 @@
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44244</v>
+        <v>44231</v>
       </c>
       <c r="B102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D102" t="n">
-        <v>166.7857993805099</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44245</v>
+        <v>44232</v>
       </c>
       <c r="B103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C103" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D103" t="n">
-        <v>262.091970455087</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44246</v>
+        <v>44233</v>
       </c>
       <c r="B104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C104" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D104" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44247</v>
+        <v>44234</v>
       </c>
       <c r="B105" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C105" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D105" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44248</v>
+        <v>44235</v>
       </c>
       <c r="B106" t="n">
+        <v>2</v>
+      </c>
+      <c r="C106" t="n">
         <v>4</v>
       </c>
-      <c r="C106" t="n">
-        <v>10</v>
-      </c>
       <c r="D106" t="n">
-        <v>238.2654276864427</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44249</v>
+        <v>44236</v>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D107" t="n">
-        <v>262.091970455087</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44250</v>
+        <v>44237</v>
       </c>
       <c r="B108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D108" t="n">
-        <v>285.9185132237312</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44251</v>
+        <v>44238</v>
       </c>
       <c r="B109" t="n">
         <v>0</v>
       </c>
       <c r="C109" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D109" t="n">
-        <v>238.2654276864427</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44252</v>
+        <v>44239</v>
       </c>
       <c r="B110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D110" t="n">
-        <v>190.6123421491542</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44253</v>
+        <v>44240</v>
       </c>
       <c r="B111" t="n">
+        <v>0</v>
+      </c>
+      <c r="C111" t="n">
         <v>3</v>
       </c>
-      <c r="C111" t="n">
-        <v>12</v>
-      </c>
       <c r="D111" t="n">
-        <v>285.9185132237312</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44254</v>
+        <v>44241</v>
       </c>
       <c r="B112" t="n">
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D112" t="n">
-        <v>285.9185132237312</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44255</v>
+        <v>44242</v>
       </c>
       <c r="B113" t="n">
         <v>2</v>
       </c>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
+      <c r="C113" t="n">
+        <v>3</v>
+      </c>
+      <c r="D113" t="n">
+        <v>71.47962830593281</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44256</v>
+        <v>44243</v>
       </c>
       <c r="B114" t="n">
+        <v>1</v>
+      </c>
+      <c r="C114" t="n">
         <v>5</v>
       </c>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr"/>
+      <c r="D114" t="n">
+        <v>119.1327138432213</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
+        <v>44244</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0</v>
+      </c>
+      <c r="C115" t="n">
+        <v>7</v>
+      </c>
+      <c r="D115" t="n">
+        <v>166.7857993805099</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0</v>
+      </c>
+      <c r="C116" t="n">
+        <v>11</v>
+      </c>
+      <c r="D116" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>44246</v>
+      </c>
+      <c r="B117" t="n">
+        <v>2</v>
+      </c>
+      <c r="C117" t="n">
+        <v>10</v>
+      </c>
+      <c r="D117" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B118" t="n">
+        <v>2</v>
+      </c>
+      <c r="C118" t="n">
+        <v>10</v>
+      </c>
+      <c r="D118" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B119" t="n">
+        <v>4</v>
+      </c>
+      <c r="C119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D119" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B120" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" t="n">
+        <v>11</v>
+      </c>
+      <c r="D120" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>44250</v>
+      </c>
+      <c r="B121" t="n">
+        <v>1</v>
+      </c>
+      <c r="C121" t="n">
+        <v>12</v>
+      </c>
+      <c r="D121" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0</v>
+      </c>
+      <c r="C122" t="n">
+        <v>10</v>
+      </c>
+      <c r="D122" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B123" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" t="n">
+        <v>8</v>
+      </c>
+      <c r="D123" t="n">
+        <v>190.6123421491542</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B124" t="n">
+        <v>3</v>
+      </c>
+      <c r="C124" t="n">
+        <v>12</v>
+      </c>
+      <c r="D124" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B125" t="n">
+        <v>0</v>
+      </c>
+      <c r="C125" t="n">
+        <v>12</v>
+      </c>
+      <c r="D125" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B126" t="n">
+        <v>2</v>
+      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B127" t="n">
+        <v>5</v>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
         <v>44257</v>
       </c>
-      <c r="B115" t="n">
-        <v>1</v>
-      </c>
-      <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr"/>
+      <c r="B128" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
ultime immagini trascritte, report aggiornati
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,7 +505,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44107</v>
+        <v>44106</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44108</v>
+        <v>44107</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44109</v>
+        <v>44108</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -547,7 +547,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44110</v>
+        <v>44109</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44111</v>
+        <v>44110</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44113</v>
+        <v>44111</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44114</v>
+        <v>44113</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -603,21 +603,21 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44115</v>
+        <v>44114</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44116</v>
+        <v>44115</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44118</v>
+        <v>44116</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -645,10 +645,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44119</v>
+        <v>44118</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44120</v>
+        <v>44119</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>2</v>
@@ -673,360 +673,360 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>142.9592566118656</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44130</v>
+        <v>44121</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D24" t="n">
-        <v>262.091970455087</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44137</v>
+        <v>44123</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D25" t="n">
-        <v>405.0512270669526</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44139</v>
+        <v>44130</v>
       </c>
       <c r="B26" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n">
-        <v>428.8777698355968</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44144</v>
+        <v>44137</v>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D27" t="n">
-        <v>476.5308553728854</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44145</v>
+        <v>44139</v>
       </c>
       <c r="B28" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D28" t="n">
-        <v>619.490111984751</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44151</v>
+        <v>44144</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D29" t="n">
-        <v>595.6635692161067</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44152</v>
+        <v>44145</v>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D30" t="n">
-        <v>571.8370264474624</v>
+        <v>619.490111984751</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44153</v>
+        <v>44151</v>
       </c>
       <c r="B31" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D31" t="n">
-        <v>548.0104836788182</v>
+        <v>595.6635692161067</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44154</v>
+        <v>44152</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D32" t="n">
-        <v>452.7043126042411</v>
+        <v>571.8370264474624</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44155</v>
+        <v>44153</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C33" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D33" t="n">
-        <v>476.5308553728854</v>
+        <v>548.0104836788182</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44156</v>
+        <v>44154</v>
       </c>
       <c r="B34" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D34" t="n">
-        <v>524.183940910174</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44157</v>
+        <v>44155</v>
       </c>
       <c r="B35" t="n">
         <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D35" t="n">
-        <v>428.8777698355968</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44158</v>
+        <v>44156</v>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D36" t="n">
-        <v>500.3573981415297</v>
+        <v>524.183940910174</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44159</v>
+        <v>44157</v>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D37" t="n">
-        <v>476.5308553728854</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44160</v>
+        <v>44158</v>
       </c>
       <c r="B38" t="n">
         <v>2</v>
       </c>
       <c r="C38" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D38" t="n">
-        <v>405.0512270669526</v>
+        <v>500.3573981415297</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44162</v>
+        <v>44159</v>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D39" t="n">
-        <v>357.398141529664</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44163</v>
+        <v>44160</v>
       </c>
       <c r="B40" t="n">
         <v>2</v>
       </c>
       <c r="C40" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D40" t="n">
-        <v>333.5715987610197</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44164</v>
+        <v>44162</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C41" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D41" t="n">
-        <v>238.2654276864427</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44165</v>
+        <v>44163</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D42" t="n">
-        <v>214.4388849177984</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44166</v>
+        <v>44164</v>
       </c>
       <c r="B43" t="n">
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D43" t="n">
-        <v>166.7857993805099</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44167</v>
+        <v>44165</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D44" t="n">
-        <v>262.091970455087</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44168</v>
+        <v>44166</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D45" t="n">
-        <v>333.5715987610197</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44169</v>
+        <v>44167</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D46" t="n">
-        <v>309.7450559923755</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44170</v>
+        <v>44168</v>
       </c>
       <c r="B47" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D47" t="n">
-        <v>309.7450559923755</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44172</v>
+        <v>44169</v>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
         <v>14</v>
@@ -1037,217 +1037,217 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44173</v>
+        <v>44170</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C49" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" t="n">
-        <v>357.398141529664</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44174</v>
+        <v>44172</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D50" t="n">
-        <v>452.7043126042411</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44175</v>
+        <v>44173</v>
       </c>
       <c r="B51" t="n">
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D51" t="n">
-        <v>428.8777698355968</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44176</v>
+        <v>44174</v>
       </c>
       <c r="B52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D52" t="n">
-        <v>357.398141529664</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44177</v>
+        <v>44175</v>
       </c>
       <c r="B53" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D53" t="n">
-        <v>428.8777698355968</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44178</v>
+        <v>44176</v>
       </c>
       <c r="B54" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C54" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D54" t="n">
-        <v>405.0512270669526</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44179</v>
+        <v>44177</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D55" t="n">
-        <v>476.5308553728854</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>44180</v>
+        <v>44178</v>
       </c>
       <c r="B56" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C56" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D56" t="n">
-        <v>476.5308553728854</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>44181</v>
+        <v>44179</v>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D57" t="n">
-        <v>428.8777698355968</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>44182</v>
+        <v>44180</v>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D58" t="n">
-        <v>309.7450559923755</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>44183</v>
+        <v>44181</v>
       </c>
       <c r="B59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D59" t="n">
-        <v>285.9185132237312</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>44184</v>
+        <v>44182</v>
       </c>
       <c r="B60" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D60" t="n">
-        <v>214.4388849177984</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>44185</v>
+        <v>44183</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C61" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D61" t="n">
-        <v>214.4388849177984</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>44187</v>
+        <v>44184</v>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C62" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D62" t="n">
-        <v>166.7857993805099</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>44188</v>
+        <v>44185</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D63" t="n">
-        <v>190.6123421491542</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>44189</v>
+        <v>44186</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
@@ -1261,217 +1261,217 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>44190</v>
+        <v>44187</v>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>44192</v>
+        <v>44188</v>
       </c>
       <c r="B66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D66" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>44194</v>
+        <v>44189</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D67" t="n">
-        <v>285.9185132237312</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>44195</v>
+        <v>44190</v>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D68" t="n">
-        <v>285.9185132237312</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44196</v>
+        <v>44192</v>
       </c>
       <c r="B69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D69" t="n">
-        <v>262.091970455087</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44197</v>
+        <v>44194</v>
       </c>
       <c r="B70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D70" t="n">
-        <v>190.6123421491542</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>44198</v>
+        <v>44195</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D71" t="n">
-        <v>238.2654276864427</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>44199</v>
+        <v>44196</v>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C72" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D72" t="n">
-        <v>238.2654276864427</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>44200</v>
+        <v>44197</v>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C73" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D73" t="n">
-        <v>142.9592566118656</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>44201</v>
+        <v>44198</v>
       </c>
       <c r="B74" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D74" t="n">
-        <v>119.1327138432213</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>44204</v>
+        <v>44199</v>
       </c>
       <c r="B75" t="n">
         <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D75" t="n">
-        <v>142.9592566118656</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>44205</v>
+        <v>44200</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>44206</v>
+        <v>44201</v>
       </c>
       <c r="B77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>44207</v>
+        <v>44204</v>
       </c>
       <c r="B78" t="n">
         <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D78" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>44208</v>
+        <v>44205</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D79" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>44209</v>
+        <v>44206</v>
       </c>
       <c r="B80" t="n">
         <v>1</v>
@@ -1485,24 +1485,24 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>44210</v>
+        <v>44207</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D81" t="n">
-        <v>142.9592566118656</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>44211</v>
+        <v>44208</v>
       </c>
       <c r="B82" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C82" t="n">
         <v>6</v>
@@ -1513,161 +1513,161 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>44212</v>
+        <v>44209</v>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D83" t="n">
-        <v>190.6123421491542</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>44213</v>
+        <v>44210</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D84" t="n">
-        <v>166.7857993805099</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>44214</v>
+        <v>44211</v>
       </c>
       <c r="B85" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>166.7857993805099</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>44215</v>
+        <v>44212</v>
       </c>
       <c r="B86" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D86" t="n">
-        <v>95.30617107457708</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>44216</v>
+        <v>44213</v>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D87" t="n">
-        <v>142.9592566118656</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>44217</v>
+        <v>44214</v>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D88" t="n">
-        <v>119.1327138432213</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>44218</v>
+        <v>44215</v>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D89" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>44219</v>
+        <v>44216</v>
       </c>
       <c r="B90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D90" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>44220</v>
+        <v>44217</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D91" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>44221</v>
+        <v>44218</v>
       </c>
       <c r="B92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D92" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44222</v>
+        <v>44219</v>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C93" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D93" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44223</v>
+        <v>44220</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
@@ -1681,52 +1681,52 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44224</v>
+        <v>44221</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95" t="n">
-        <v>95.30617107457708</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44225</v>
+        <v>44222</v>
       </c>
       <c r="B96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D96" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44226</v>
+        <v>44223</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D97" t="n">
-        <v>95.30617107457708</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44227</v>
+        <v>44224</v>
       </c>
       <c r="B98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" t="n">
         <v>4</v>
@@ -1737,24 +1737,24 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44228</v>
+        <v>44225</v>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C99" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D99" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44229</v>
+        <v>44226</v>
       </c>
       <c r="B100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" t="n">
         <v>4</v>
@@ -1765,52 +1765,52 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44230</v>
+        <v>44227</v>
       </c>
       <c r="B101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D101" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44231</v>
+        <v>44228</v>
       </c>
       <c r="B102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D102" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44232</v>
+        <v>44229</v>
       </c>
       <c r="B103" t="n">
         <v>1</v>
       </c>
       <c r="C103" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D103" t="n">
-        <v>142.9592566118656</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44233</v>
+        <v>44230</v>
       </c>
       <c r="B104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" t="n">
         <v>5</v>
@@ -1821,248 +1821,248 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44234</v>
+        <v>44231</v>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D105" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44235</v>
+        <v>44232</v>
       </c>
       <c r="B106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D106" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44236</v>
+        <v>44233</v>
       </c>
       <c r="B107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C107" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D107" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44237</v>
+        <v>44234</v>
       </c>
       <c r="B108" t="n">
         <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D108" t="n">
-        <v>47.65308553728854</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44238</v>
+        <v>44235</v>
       </c>
       <c r="B109" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C109" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D109" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44239</v>
+        <v>44236</v>
       </c>
       <c r="B110" t="n">
         <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D110" t="n">
-        <v>47.65308553728854</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44240</v>
+        <v>44237</v>
       </c>
       <c r="B111" t="n">
         <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D111" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44241</v>
+        <v>44238</v>
       </c>
       <c r="B112" t="n">
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D112" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44242</v>
+        <v>44239</v>
       </c>
       <c r="B113" t="n">
+        <v>0</v>
+      </c>
+      <c r="C113" t="n">
         <v>2</v>
       </c>
-      <c r="C113" t="n">
-        <v>3</v>
-      </c>
       <c r="D113" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44243</v>
+        <v>44240</v>
       </c>
       <c r="B114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D114" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44244</v>
+        <v>44241</v>
       </c>
       <c r="B115" t="n">
         <v>0</v>
       </c>
       <c r="C115" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D115" t="n">
-        <v>166.7857993805099</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44245</v>
+        <v>44242</v>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C116" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D116" t="n">
-        <v>262.091970455087</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44246</v>
+        <v>44243</v>
       </c>
       <c r="B117" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C117" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D117" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44247</v>
+        <v>44244</v>
       </c>
       <c r="B118" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C118" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D118" t="n">
-        <v>238.2654276864427</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44248</v>
+        <v>44245</v>
       </c>
       <c r="B119" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C119" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D119" t="n">
-        <v>238.2654276864427</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44249</v>
+        <v>44246</v>
       </c>
       <c r="B120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C120" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D120" t="n">
-        <v>262.091970455087</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44250</v>
+        <v>44247</v>
       </c>
       <c r="B121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C121" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D121" t="n">
-        <v>285.9185132237312</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44251</v>
+        <v>44248</v>
       </c>
       <c r="B122" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C122" t="n">
         <v>10</v>
@@ -2073,24 +2073,24 @@
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>44252</v>
+        <v>44249</v>
       </c>
       <c r="B123" t="n">
         <v>1</v>
       </c>
       <c r="C123" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D123" t="n">
-        <v>190.6123421491542</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>44253</v>
+        <v>44250</v>
       </c>
       <c r="B124" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C124" t="n">
         <v>12</v>
@@ -2101,47 +2101,89 @@
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>44254</v>
+        <v>44251</v>
       </c>
       <c r="B125" t="n">
         <v>0</v>
       </c>
       <c r="C125" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D125" t="n">
-        <v>285.9185132237312</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>44255</v>
+        <v>44252</v>
       </c>
       <c r="B126" t="n">
-        <v>2</v>
-      </c>
-      <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="C126" t="n">
+        <v>8</v>
+      </c>
+      <c r="D126" t="n">
+        <v>190.6123421491542</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>44256</v>
+        <v>44253</v>
       </c>
       <c r="B127" t="n">
-        <v>5</v>
-      </c>
-      <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="C127" t="n">
+        <v>12</v>
+      </c>
+      <c r="D127" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B128" t="n">
+        <v>0</v>
+      </c>
+      <c r="C128" t="n">
+        <v>12</v>
+      </c>
+      <c r="D128" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B129" t="n">
+        <v>2</v>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B130" t="n">
+        <v>5</v>
+      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
         <v>44257</v>
       </c>
-      <c r="B128" t="n">
-        <v>1</v>
-      </c>
-      <c r="C128" t="inlineStr"/>
-      <c r="D128" t="inlineStr"/>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
aggiunti altri giorni, aggiornati report
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,10 +707,10 @@
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>166.7857993805099</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="26">
@@ -721,71 +721,71 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>262.091970455087</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44137</v>
+        <v>44136</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D27" t="n">
-        <v>428.8777698355968</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44139</v>
+        <v>44137</v>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D28" t="n">
-        <v>452.7043126042411</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44144</v>
+        <v>44138</v>
       </c>
       <c r="B29" t="n">
         <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D29" t="n">
-        <v>476.5308553728854</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44145</v>
+        <v>44139</v>
       </c>
       <c r="B30" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D30" t="n">
-        <v>619.490111984751</v>
+        <v>500.3573981415297</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44151</v>
+        <v>44141</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
@@ -799,276 +799,276 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44152</v>
+        <v>44142</v>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D32" t="n">
-        <v>571.8370264474624</v>
+        <v>738.6228258279724</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44153</v>
+        <v>44143</v>
       </c>
       <c r="B33" t="n">
         <v>6</v>
       </c>
       <c r="C33" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D33" t="n">
-        <v>548.0104836788182</v>
+        <v>667.1431975220395</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44154</v>
+        <v>44144</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D34" t="n">
-        <v>452.7043126042411</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44155</v>
+        <v>44145</v>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C35" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D35" t="n">
-        <v>476.5308553728854</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44156</v>
+        <v>44146</v>
       </c>
       <c r="B36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>524.183940910174</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44157</v>
+        <v>44147</v>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C37" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D37" t="n">
-        <v>428.8777698355968</v>
+        <v>810.1024541339052</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44158</v>
+        <v>44148</v>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D38" t="n">
-        <v>500.3573981415297</v>
+        <v>714.7962830593281</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44159</v>
+        <v>44149</v>
       </c>
       <c r="B39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D39" t="n">
-        <v>476.5308553728854</v>
+        <v>595.6635692161067</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44160</v>
+        <v>44150</v>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C40" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D40" t="n">
-        <v>405.0512270669526</v>
+        <v>690.9697402906838</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44162</v>
+        <v>44151</v>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D41" t="n">
-        <v>357.398141529664</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44163</v>
+        <v>44152</v>
       </c>
       <c r="B42" t="n">
         <v>2</v>
       </c>
       <c r="C42" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D42" t="n">
-        <v>333.5715987610197</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44164</v>
+        <v>44153</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C43" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D43" t="n">
-        <v>238.2654276864427</v>
+        <v>500.3573981415297</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44165</v>
+        <v>44154</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D44" t="n">
-        <v>214.4388849177984</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44166</v>
+        <v>44155</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D45" t="n">
-        <v>166.7857993805099</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44167</v>
+        <v>44156</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D46" t="n">
-        <v>262.091970455087</v>
+        <v>524.183940910174</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44168</v>
+        <v>44157</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D47" t="n">
-        <v>333.5715987610197</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44169</v>
+        <v>44158</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D48" t="n">
-        <v>333.5715987610197</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44170</v>
+        <v>44159</v>
       </c>
       <c r="B49" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D49" t="n">
-        <v>333.5715987610197</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44172</v>
+        <v>44160</v>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D50" t="n">
-        <v>357.398141529664</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44173</v>
+        <v>44161</v>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" t="n">
         <v>16</v>
@@ -1079,122 +1079,122 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44174</v>
+        <v>44162</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C52" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D52" t="n">
-        <v>476.5308553728854</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44175</v>
+        <v>44163</v>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D53" t="n">
-        <v>452.7043126042411</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44176</v>
+        <v>44164</v>
       </c>
       <c r="B54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D54" t="n">
-        <v>381.2246842983083</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44177</v>
+        <v>44165</v>
       </c>
       <c r="B55" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D55" t="n">
-        <v>428.8777698355968</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>44178</v>
+        <v>44166</v>
       </c>
       <c r="B56" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D56" t="n">
-        <v>405.0512270669526</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>44179</v>
+        <v>44167</v>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D57" t="n">
-        <v>476.5308553728854</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>44180</v>
+        <v>44168</v>
       </c>
       <c r="B58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D58" t="n">
-        <v>476.5308553728854</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>44181</v>
+        <v>44169</v>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D59" t="n">
-        <v>428.8777698355968</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>44182</v>
+        <v>44170</v>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C60" t="n">
         <v>13</v>
@@ -1205,234 +1205,234 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>44183</v>
+        <v>44171</v>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D61" t="n">
-        <v>285.9185132237312</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>44184</v>
+        <v>44172</v>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C62" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D62" t="n">
-        <v>214.4388849177984</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>44185</v>
+        <v>44173</v>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D63" t="n">
-        <v>214.4388849177984</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>44186</v>
+        <v>44174</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D64" t="n">
-        <v>119.1327138432213</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>44187</v>
+        <v>44175</v>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D65" t="n">
-        <v>119.1327138432213</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>44188</v>
+        <v>44176</v>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C66" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D66" t="n">
-        <v>119.1327138432213</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>44189</v>
+        <v>44177</v>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C67" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D67" t="n">
-        <v>119.1327138432213</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>44190</v>
+        <v>44178</v>
       </c>
       <c r="B68" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D68" t="n">
-        <v>142.9592566118656</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44192</v>
+        <v>44179</v>
       </c>
       <c r="B69" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D69" t="n">
-        <v>238.2654276864427</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44194</v>
+        <v>44180</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D70" t="n">
-        <v>285.9185132237312</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>44195</v>
+        <v>44181</v>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D71" t="n">
-        <v>285.9185132237312</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>44196</v>
+        <v>44182</v>
       </c>
       <c r="B72" t="n">
         <v>4</v>
       </c>
       <c r="C72" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D72" t="n">
-        <v>262.091970455087</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>44197</v>
+        <v>44183</v>
       </c>
       <c r="B73" t="n">
         <v>2</v>
       </c>
       <c r="C73" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D73" t="n">
-        <v>190.6123421491542</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>44198</v>
+        <v>44184</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D74" t="n">
-        <v>238.2654276864427</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>44199</v>
+        <v>44185</v>
       </c>
       <c r="B75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D75" t="n">
-        <v>238.2654276864427</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>44200</v>
+        <v>44186</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D76" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>44201</v>
+        <v>44187</v>
       </c>
       <c r="B77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C77" t="n">
         <v>5</v>
@@ -1443,38 +1443,38 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>44204</v>
+        <v>44188</v>
       </c>
       <c r="B78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D78" t="n">
-        <v>142.9592566118656</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>44205</v>
+        <v>44189</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>44206</v>
+        <v>44190</v>
       </c>
       <c r="B80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C80" t="n">
         <v>6</v>
@@ -1485,80 +1485,80 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>44207</v>
+        <v>44191</v>
       </c>
       <c r="B81" t="n">
         <v>1</v>
       </c>
       <c r="C81" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D81" t="n">
-        <v>95.30617107457708</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>44208</v>
+        <v>44192</v>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C82" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D82" t="n">
-        <v>142.9592566118656</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>44209</v>
+        <v>44194</v>
       </c>
       <c r="B83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D83" t="n">
-        <v>142.9592566118656</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>44210</v>
+        <v>44195</v>
       </c>
       <c r="B84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D84" t="n">
-        <v>142.9592566118656</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>44211</v>
+        <v>44196</v>
       </c>
       <c r="B85" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C85" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D85" t="n">
-        <v>142.9592566118656</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>44212</v>
+        <v>44197</v>
       </c>
       <c r="B86" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C86" t="n">
         <v>8</v>
@@ -1569,234 +1569,234 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>44213</v>
+        <v>44198</v>
       </c>
       <c r="B87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D87" t="n">
-        <v>166.7857993805099</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>44214</v>
+        <v>44199</v>
       </c>
       <c r="B88" t="n">
         <v>1</v>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D88" t="n">
-        <v>166.7857993805099</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>44215</v>
+        <v>44200</v>
       </c>
       <c r="B89" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D89" t="n">
-        <v>95.30617107457708</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>44216</v>
+        <v>44201</v>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D90" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>44217</v>
+        <v>44203</v>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D91" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>44218</v>
+        <v>44204</v>
       </c>
       <c r="B92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D92" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44219</v>
+        <v>44205</v>
       </c>
       <c r="B93" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D93" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44220</v>
+        <v>44206</v>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D94" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44221</v>
+        <v>44207</v>
       </c>
       <c r="B95" t="n">
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D95" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44222</v>
+        <v>44208</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D96" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44223</v>
+        <v>44209</v>
       </c>
       <c r="B97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D97" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44224</v>
+        <v>44210</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D98" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44225</v>
+        <v>44211</v>
       </c>
       <c r="B99" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C99" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D99" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44226</v>
+        <v>44212</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D100" t="n">
-        <v>95.30617107457708</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44227</v>
+        <v>44213</v>
       </c>
       <c r="B101" t="n">
         <v>1</v>
       </c>
       <c r="C101" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D101" t="n">
-        <v>95.30617107457708</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44228</v>
+        <v>44214</v>
       </c>
       <c r="B102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D102" t="n">
-        <v>119.1327138432213</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44229</v>
+        <v>44215</v>
       </c>
       <c r="B103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C103" t="n">
         <v>4</v>
@@ -1807,383 +1807,579 @@
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44230</v>
+        <v>44216</v>
       </c>
       <c r="B104" t="n">
         <v>0</v>
       </c>
       <c r="C104" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D104" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44231</v>
+        <v>44217</v>
       </c>
       <c r="B105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D105" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44232</v>
+        <v>44218</v>
       </c>
       <c r="B106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D106" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44233</v>
+        <v>44219</v>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C107" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D107" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44234</v>
+        <v>44220</v>
       </c>
       <c r="B108" t="n">
         <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D108" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44235</v>
+        <v>44221</v>
       </c>
       <c r="B109" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C109" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D109" t="n">
-        <v>95.30617107457708</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44236</v>
+        <v>44222</v>
       </c>
       <c r="B110" t="n">
         <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D110" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44237</v>
+        <v>44223</v>
       </c>
       <c r="B111" t="n">
         <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D111" t="n">
-        <v>47.65308553728854</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44238</v>
+        <v>44224</v>
       </c>
       <c r="B112" t="n">
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D112" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44239</v>
+        <v>44225</v>
       </c>
       <c r="B113" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C113" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D113" t="n">
-        <v>47.65308553728854</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44240</v>
+        <v>44226</v>
       </c>
       <c r="B114" t="n">
         <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D114" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44241</v>
+        <v>44227</v>
       </c>
       <c r="B115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D115" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44242</v>
+        <v>44228</v>
       </c>
       <c r="B116" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D116" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44243</v>
+        <v>44229</v>
       </c>
       <c r="B117" t="n">
         <v>1</v>
       </c>
       <c r="C117" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D117" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44244</v>
+        <v>44230</v>
       </c>
       <c r="B118" t="n">
         <v>0</v>
       </c>
       <c r="C118" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D118" t="n">
-        <v>166.7857993805099</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44245</v>
+        <v>44231</v>
       </c>
       <c r="B119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C119" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D119" t="n">
-        <v>262.091970455087</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44246</v>
+        <v>44232</v>
       </c>
       <c r="B120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C120" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D120" t="n">
-        <v>238.2654276864427</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44247</v>
+        <v>44233</v>
       </c>
       <c r="B121" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C121" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D121" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44248</v>
+        <v>44234</v>
       </c>
       <c r="B122" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D122" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>44249</v>
+        <v>44235</v>
       </c>
       <c r="B123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C123" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D123" t="n">
-        <v>262.091970455087</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>44250</v>
+        <v>44236</v>
       </c>
       <c r="B124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D124" t="n">
-        <v>285.9185132237312</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>44251</v>
+        <v>44237</v>
       </c>
       <c r="B125" t="n">
         <v>0</v>
       </c>
       <c r="C125" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D125" t="n">
-        <v>238.2654276864427</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>44252</v>
+        <v>44238</v>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C126" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D126" t="n">
-        <v>190.6123421491542</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>44253</v>
+        <v>44239</v>
       </c>
       <c r="B127" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C127" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D127" t="n">
-        <v>285.9185132237312</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>44254</v>
+        <v>44240</v>
       </c>
       <c r="B128" t="n">
         <v>0</v>
       </c>
       <c r="C128" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D128" t="n">
-        <v>285.9185132237312</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>44255</v>
+        <v>44241</v>
       </c>
       <c r="B129" t="n">
-        <v>2</v>
-      </c>
-      <c r="C129" t="inlineStr"/>
-      <c r="D129" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C129" t="n">
+        <v>3</v>
+      </c>
+      <c r="D129" t="n">
+        <v>71.47962830593281</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>44256</v>
+        <v>44242</v>
       </c>
       <c r="B130" t="n">
-        <v>5</v>
-      </c>
-      <c r="C130" t="inlineStr"/>
-      <c r="D130" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="C130" t="n">
+        <v>3</v>
+      </c>
+      <c r="D130" t="n">
+        <v>71.47962830593281</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" t="n">
+        <v>5</v>
+      </c>
+      <c r="D131" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>44244</v>
+      </c>
+      <c r="B132" t="n">
+        <v>0</v>
+      </c>
+      <c r="C132" t="n">
+        <v>7</v>
+      </c>
+      <c r="D132" t="n">
+        <v>166.7857993805099</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B133" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" t="n">
+        <v>11</v>
+      </c>
+      <c r="D133" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>44246</v>
+      </c>
+      <c r="B134" t="n">
+        <v>2</v>
+      </c>
+      <c r="C134" t="n">
+        <v>10</v>
+      </c>
+      <c r="D134" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B135" t="n">
+        <v>2</v>
+      </c>
+      <c r="C135" t="n">
+        <v>10</v>
+      </c>
+      <c r="D135" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B136" t="n">
+        <v>4</v>
+      </c>
+      <c r="C136" t="n">
+        <v>10</v>
+      </c>
+      <c r="D136" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+      <c r="C137" t="n">
+        <v>11</v>
+      </c>
+      <c r="D137" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>44250</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+      <c r="C138" t="n">
+        <v>12</v>
+      </c>
+      <c r="D138" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B139" t="n">
+        <v>0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>10</v>
+      </c>
+      <c r="D139" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+      <c r="C140" t="n">
+        <v>8</v>
+      </c>
+      <c r="D140" t="n">
+        <v>190.6123421491542</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B141" t="n">
+        <v>3</v>
+      </c>
+      <c r="C141" t="n">
+        <v>12</v>
+      </c>
+      <c r="D141" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B142" t="n">
+        <v>0</v>
+      </c>
+      <c r="C142" t="n">
+        <v>12</v>
+      </c>
+      <c r="D142" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B143" t="n">
+        <v>2</v>
+      </c>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B144" t="n">
+        <v>5</v>
+      </c>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
         <v>44257</v>
       </c>
-      <c r="B131" t="n">
-        <v>1</v>
-      </c>
-      <c r="C131" t="inlineStr"/>
-      <c r="D131" t="inlineStr"/>
+      <c r="B145" t="n">
+        <v>1</v>
+      </c>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
aggiornati tutti i giorni da 1 sett a oggi, mancano solo 6 gennaio e 28 dicembre
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,17 +391,17 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44087</v>
+        <v>44075</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44088</v>
+        <v>44076</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -411,7 +411,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44089</v>
+        <v>44077</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -421,21 +421,21 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44094</v>
+        <v>44078</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44095</v>
+        <v>44079</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44097</v>
+        <v>44080</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44100</v>
+        <v>44081</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44101</v>
+        <v>44082</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44102</v>
+        <v>44083</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -505,119 +505,119 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44106</v>
+        <v>44084</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44107</v>
+        <v>44085</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44108</v>
+        <v>44086</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44109</v>
+        <v>44087</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44110</v>
+        <v>44088</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44111</v>
+        <v>44089</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44113</v>
+        <v>44090</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44114</v>
+        <v>44091</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44115</v>
+        <v>44092</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44116</v>
+        <v>44093</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -645,595 +645,595 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44118</v>
+        <v>44094</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44119</v>
+        <v>44095</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>47.65308553728854</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44120</v>
+        <v>44096</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>47.65308553728854</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44121</v>
+        <v>44097</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>71.47962830593281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44123</v>
+        <v>44098</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>95.30617107457708</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44130</v>
+        <v>44099</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>190.6123421491542</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44136</v>
+        <v>44100</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>285.9185132237312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44137</v>
+        <v>44101</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>309.7450559923755</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44138</v>
+        <v>44102</v>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>357.398141529664</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44139</v>
+        <v>44103</v>
       </c>
       <c r="B30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>500.3573981415297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44141</v>
+        <v>44104</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>595.6635692161067</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44142</v>
+        <v>44105</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>738.6228258279724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44143</v>
+        <v>44106</v>
       </c>
       <c r="B33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>667.1431975220395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44144</v>
+        <v>44107</v>
       </c>
       <c r="B34" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>833.9289969025494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44145</v>
+        <v>44108</v>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>833.9289969025494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44146</v>
+        <v>44109</v>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>833.9289969025494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44147</v>
+        <v>44110</v>
       </c>
       <c r="B37" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>810.1024541339052</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44148</v>
+        <v>44111</v>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>714.7962830593281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44149</v>
+        <v>44112</v>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>595.6635692161067</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44150</v>
+        <v>44113</v>
       </c>
       <c r="B40" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>690.9697402906838</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44151</v>
+        <v>44114</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>428.8777698355968</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44152</v>
+        <v>44115</v>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>476.5308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44153</v>
+        <v>44116</v>
       </c>
       <c r="B43" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>500.3573981415297</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44154</v>
+        <v>44117</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>452.7043126042411</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44155</v>
+        <v>44118</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>476.5308553728854</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44156</v>
+        <v>44119</v>
       </c>
       <c r="B46" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" t="n">
         <v>4</v>
       </c>
-      <c r="C46" t="n">
-        <v>22</v>
-      </c>
       <c r="D46" t="n">
-        <v>524.183940910174</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44157</v>
+        <v>44120</v>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D47" t="n">
-        <v>428.8777698355968</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44158</v>
+        <v>44121</v>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D48" t="n">
-        <v>476.5308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44159</v>
+        <v>44122</v>
       </c>
       <c r="B49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D49" t="n">
-        <v>476.5308553728854</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44160</v>
+        <v>44123</v>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D50" t="n">
-        <v>428.8777698355968</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44161</v>
+        <v>44124</v>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D51" t="n">
-        <v>381.2246842983083</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44162</v>
+        <v>44125</v>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D52" t="n">
-        <v>357.398141529664</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44163</v>
+        <v>44126</v>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D53" t="n">
-        <v>285.9185132237312</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44164</v>
+        <v>44127</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D54" t="n">
-        <v>238.2654276864427</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44165</v>
+        <v>44128</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D55" t="n">
-        <v>214.4388849177984</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>44166</v>
+        <v>44129</v>
       </c>
       <c r="B56" t="n">
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
-        <v>166.7857993805099</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>44167</v>
+        <v>44130</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D57" t="n">
-        <v>262.091970455087</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>44168</v>
+        <v>44131</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D58" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>44169</v>
+        <v>44132</v>
       </c>
       <c r="B59" t="n">
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D59" t="n">
-        <v>309.7450559923755</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>44170</v>
+        <v>44133</v>
       </c>
       <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
         <v>6</v>
       </c>
-      <c r="C60" t="n">
-        <v>13</v>
-      </c>
       <c r="D60" t="n">
-        <v>309.7450559923755</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>44171</v>
+        <v>44134</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C61" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D61" t="n">
-        <v>333.5715987610197</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>44172</v>
+        <v>44135</v>
       </c>
       <c r="B62" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D62" t="n">
-        <v>333.5715987610197</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>44173</v>
+        <v>44136</v>
       </c>
       <c r="B63" t="n">
         <v>1</v>
@@ -1247,945 +1247,945 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>44174</v>
+        <v>44137</v>
       </c>
       <c r="B64" t="n">
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D64" t="n">
-        <v>333.5715987610197</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>44175</v>
+        <v>44138</v>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C65" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D65" t="n">
-        <v>452.7043126042411</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>44176</v>
+        <v>44139</v>
       </c>
       <c r="B66" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C66" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D66" t="n">
-        <v>381.2246842983083</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>44177</v>
+        <v>44140</v>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C67" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D67" t="n">
-        <v>428.8777698355968</v>
+        <v>548.0104836788182</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>44178</v>
+        <v>44141</v>
       </c>
       <c r="B68" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D68" t="n">
-        <v>405.0512270669526</v>
+        <v>643.3166547533953</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44179</v>
+        <v>44142</v>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D69" t="n">
-        <v>476.5308553728854</v>
+        <v>690.9697402906838</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44180</v>
+        <v>44143</v>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C70" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D70" t="n">
-        <v>476.5308553728854</v>
+        <v>643.3166547533953</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>44181</v>
+        <v>44144</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C71" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D71" t="n">
-        <v>428.8777698355968</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>44182</v>
+        <v>44145</v>
       </c>
       <c r="B72" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C72" t="n">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D72" t="n">
-        <v>309.7450559923755</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>44183</v>
+        <v>44146</v>
       </c>
       <c r="B73" t="n">
         <v>2</v>
       </c>
       <c r="C73" t="n">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D73" t="n">
-        <v>285.9185132237312</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>44184</v>
+        <v>44147</v>
       </c>
       <c r="B74" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C74" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D74" t="n">
-        <v>214.4388849177984</v>
+        <v>810.1024541339052</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>44185</v>
+        <v>44148</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D75" t="n">
-        <v>214.4388849177984</v>
+        <v>714.7962830593281</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>44186</v>
+        <v>44149</v>
       </c>
       <c r="B76" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D76" t="n">
-        <v>119.1327138432213</v>
+        <v>595.6635692161067</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>44187</v>
+        <v>44150</v>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C77" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D77" t="n">
-        <v>119.1327138432213</v>
+        <v>690.9697402906838</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>44188</v>
+        <v>44151</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D78" t="n">
-        <v>71.47962830593281</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>44189</v>
+        <v>44152</v>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C79" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D79" t="n">
-        <v>142.9592566118656</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>44190</v>
+        <v>44153</v>
       </c>
       <c r="B80" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C80" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D80" t="n">
-        <v>142.9592566118656</v>
+        <v>500.3573981415297</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>44191</v>
+        <v>44154</v>
       </c>
       <c r="B81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D81" t="n">
-        <v>166.7857993805099</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>44192</v>
+        <v>44155</v>
       </c>
       <c r="B82" t="n">
         <v>3</v>
       </c>
       <c r="C82" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D82" t="n">
-        <v>262.091970455087</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>44194</v>
+        <v>44156</v>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C83" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D83" t="n">
-        <v>309.7450559923755</v>
+        <v>524.183940910174</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>44195</v>
+        <v>44157</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C84" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D84" t="n">
-        <v>262.091970455087</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>44196</v>
+        <v>44158</v>
       </c>
       <c r="B85" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C85" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D85" t="n">
-        <v>262.091970455087</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>44197</v>
+        <v>44159</v>
       </c>
       <c r="B86" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C86" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D86" t="n">
-        <v>190.6123421491542</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>44198</v>
+        <v>44160</v>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C87" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D87" t="n">
-        <v>238.2654276864427</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>44199</v>
+        <v>44161</v>
       </c>
       <c r="B88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C88" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D88" t="n">
-        <v>238.2654276864427</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>44200</v>
+        <v>44162</v>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D89" t="n">
-        <v>166.7857993805099</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>44201</v>
+        <v>44163</v>
       </c>
       <c r="B90" t="n">
         <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D90" t="n">
-        <v>119.1327138432213</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>44203</v>
+        <v>44164</v>
       </c>
       <c r="B91" t="n">
         <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D91" t="n">
-        <v>142.9592566118656</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>44204</v>
+        <v>44165</v>
       </c>
       <c r="B92" t="n">
         <v>1</v>
       </c>
       <c r="C92" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D92" t="n">
-        <v>142.9592566118656</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44205</v>
+        <v>44166</v>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D93" t="n">
-        <v>142.9592566118656</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44206</v>
+        <v>44167</v>
       </c>
       <c r="B94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D94" t="n">
-        <v>119.1327138432213</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44207</v>
+        <v>44168</v>
       </c>
       <c r="B95" t="n">
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D95" t="n">
-        <v>95.30617107457708</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44208</v>
+        <v>44169</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D96" t="n">
-        <v>142.9592566118656</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44209</v>
+        <v>44170</v>
       </c>
       <c r="B97" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C97" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D97" t="n">
-        <v>142.9592566118656</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44210</v>
+        <v>44171</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D98" t="n">
-        <v>142.9592566118656</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44211</v>
+        <v>44172</v>
       </c>
       <c r="B99" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C99" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D99" t="n">
-        <v>142.9592566118656</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44212</v>
+        <v>44173</v>
       </c>
       <c r="B100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D100" t="n">
-        <v>190.6123421491542</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44213</v>
+        <v>44174</v>
       </c>
       <c r="B101" t="n">
         <v>1</v>
       </c>
       <c r="C101" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D101" t="n">
-        <v>166.7857993805099</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44214</v>
+        <v>44175</v>
       </c>
       <c r="B102" t="n">
         <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D102" t="n">
-        <v>166.7857993805099</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44215</v>
+        <v>44176</v>
       </c>
       <c r="B103" t="n">
         <v>2</v>
       </c>
       <c r="C103" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D103" t="n">
-        <v>95.30617107457708</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44216</v>
+        <v>44177</v>
       </c>
       <c r="B104" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C104" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D104" t="n">
-        <v>142.9592566118656</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44217</v>
+        <v>44178</v>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C105" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D105" t="n">
-        <v>119.1327138432213</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44218</v>
+        <v>44179</v>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D106" t="n">
-        <v>119.1327138432213</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44219</v>
+        <v>44180</v>
       </c>
       <c r="B107" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D107" t="n">
-        <v>71.47962830593281</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44220</v>
+        <v>44181</v>
       </c>
       <c r="B108" t="n">
         <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D108" t="n">
-        <v>71.47962830593281</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44221</v>
+        <v>44182</v>
       </c>
       <c r="B109" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C109" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D109" t="n">
-        <v>71.47962830593281</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44222</v>
+        <v>44183</v>
       </c>
       <c r="B110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C110" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D110" t="n">
-        <v>119.1327138432213</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44223</v>
+        <v>44184</v>
       </c>
       <c r="B111" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C111" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D111" t="n">
-        <v>71.47962830593281</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44224</v>
+        <v>44185</v>
       </c>
       <c r="B112" t="n">
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D112" t="n">
-        <v>95.30617107457708</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44225</v>
+        <v>44186</v>
       </c>
       <c r="B113" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D113" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44226</v>
+        <v>44187</v>
       </c>
       <c r="B114" t="n">
         <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D114" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44227</v>
+        <v>44188</v>
       </c>
       <c r="B115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D115" t="n">
-        <v>95.30617107457708</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44228</v>
+        <v>44189</v>
       </c>
       <c r="B116" t="n">
         <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D116" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44229</v>
+        <v>44190</v>
       </c>
       <c r="B117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C117" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44230</v>
+        <v>44191</v>
       </c>
       <c r="B118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C118" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D118" t="n">
-        <v>119.1327138432213</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44231</v>
+        <v>44192</v>
       </c>
       <c r="B119" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C119" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D119" t="n">
-        <v>95.30617107457708</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44232</v>
+        <v>44194</v>
       </c>
       <c r="B120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D120" t="n">
-        <v>142.9592566118656</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44233</v>
+        <v>44195</v>
       </c>
       <c r="B121" t="n">
         <v>1</v>
       </c>
       <c r="C121" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D121" t="n">
-        <v>119.1327138432213</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44234</v>
+        <v>44196</v>
       </c>
       <c r="B122" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C122" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D122" t="n">
-        <v>119.1327138432213</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>44235</v>
+        <v>44197</v>
       </c>
       <c r="B123" t="n">
         <v>2</v>
       </c>
       <c r="C123" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D123" t="n">
-        <v>95.30617107457708</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>44236</v>
+        <v>44198</v>
       </c>
       <c r="B124" t="n">
         <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D124" t="n">
-        <v>71.47962830593281</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>44237</v>
+        <v>44199</v>
       </c>
       <c r="B125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D125" t="n">
-        <v>47.65308553728854</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>44238</v>
+        <v>44200</v>
       </c>
       <c r="B126" t="n">
         <v>0</v>
       </c>
       <c r="C126" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D126" t="n">
-        <v>47.65308553728854</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>44239</v>
+        <v>44201</v>
       </c>
       <c r="B127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C127" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D127" t="n">
-        <v>47.65308553728854</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>44240</v>
+        <v>44203</v>
       </c>
       <c r="B128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C128" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D128" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>44241</v>
+        <v>44204</v>
       </c>
       <c r="B129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D129" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>44242</v>
+        <v>44205</v>
       </c>
       <c r="B130" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C130" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D130" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>44243</v>
+        <v>44206</v>
       </c>
       <c r="B131" t="n">
         <v>1</v>
@@ -2199,187 +2199,705 @@
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>44244</v>
+        <v>44207</v>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C132" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D132" t="n">
-        <v>166.7857993805099</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>44245</v>
+        <v>44208</v>
       </c>
       <c r="B133" t="n">
         <v>0</v>
       </c>
       <c r="C133" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D133" t="n">
-        <v>262.091970455087</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>44246</v>
+        <v>44209</v>
       </c>
       <c r="B134" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C134" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D134" t="n">
-        <v>238.2654276864427</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>44247</v>
+        <v>44210</v>
       </c>
       <c r="B135" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C135" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D135" t="n">
-        <v>238.2654276864427</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>44248</v>
+        <v>44211</v>
       </c>
       <c r="B136" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C136" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D136" t="n">
-        <v>238.2654276864427</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>44249</v>
+        <v>44212</v>
       </c>
       <c r="B137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D137" t="n">
-        <v>262.091970455087</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>44250</v>
+        <v>44213</v>
       </c>
       <c r="B138" t="n">
         <v>1</v>
       </c>
       <c r="C138" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D138" t="n">
-        <v>285.9185132237312</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>44251</v>
+        <v>44214</v>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D139" t="n">
-        <v>238.2654276864427</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>44252</v>
+        <v>44215</v>
       </c>
       <c r="B140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C140" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D140" t="n">
-        <v>190.6123421491542</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>44253</v>
+        <v>44216</v>
       </c>
       <c r="B141" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C141" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D141" t="n">
-        <v>285.9185132237312</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>44254</v>
+        <v>44217</v>
       </c>
       <c r="B142" t="n">
         <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D142" t="n">
-        <v>285.9185132237312</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>44255</v>
+        <v>44218</v>
       </c>
       <c r="B143" t="n">
-        <v>2</v>
-      </c>
-      <c r="C143" t="inlineStr"/>
-      <c r="D143" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C143" t="n">
+        <v>5</v>
+      </c>
+      <c r="D143" t="n">
+        <v>119.1327138432213</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>44256</v>
+        <v>44219</v>
       </c>
       <c r="B144" t="n">
-        <v>5</v>
-      </c>
-      <c r="C144" t="inlineStr"/>
-      <c r="D144" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="C144" t="n">
+        <v>3</v>
+      </c>
+      <c r="D144" t="n">
+        <v>71.47962830593281</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
+        <v>44220</v>
+      </c>
+      <c r="B145" t="n">
+        <v>0</v>
+      </c>
+      <c r="C145" t="n">
+        <v>3</v>
+      </c>
+      <c r="D145" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>44221</v>
+      </c>
+      <c r="B146" t="n">
+        <v>1</v>
+      </c>
+      <c r="C146" t="n">
+        <v>3</v>
+      </c>
+      <c r="D146" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B147" t="n">
+        <v>0</v>
+      </c>
+      <c r="C147" t="n">
+        <v>5</v>
+      </c>
+      <c r="D147" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>44223</v>
+      </c>
+      <c r="B148" t="n">
+        <v>0</v>
+      </c>
+      <c r="C148" t="n">
+        <v>3</v>
+      </c>
+      <c r="D148" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>44224</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+      <c r="C149" t="n">
+        <v>4</v>
+      </c>
+      <c r="D149" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>44225</v>
+      </c>
+      <c r="B150" t="n">
+        <v>2</v>
+      </c>
+      <c r="C150" t="n">
+        <v>3</v>
+      </c>
+      <c r="D150" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="n">
+        <v>44226</v>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+      <c r="C151" t="n">
+        <v>4</v>
+      </c>
+      <c r="D151" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1</v>
+      </c>
+      <c r="C152" t="n">
+        <v>4</v>
+      </c>
+      <c r="D152" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>44228</v>
+      </c>
+      <c r="B153" t="n">
+        <v>0</v>
+      </c>
+      <c r="C153" t="n">
+        <v>5</v>
+      </c>
+      <c r="D153" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B154" t="n">
+        <v>1</v>
+      </c>
+      <c r="C154" t="n">
+        <v>4</v>
+      </c>
+      <c r="D154" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="n">
+        <v>44230</v>
+      </c>
+      <c r="B155" t="n">
+        <v>0</v>
+      </c>
+      <c r="C155" t="n">
+        <v>5</v>
+      </c>
+      <c r="D155" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B156" t="n">
+        <v>1</v>
+      </c>
+      <c r="C156" t="n">
+        <v>4</v>
+      </c>
+      <c r="D156" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B157" t="n">
+        <v>1</v>
+      </c>
+      <c r="C157" t="n">
+        <v>6</v>
+      </c>
+      <c r="D157" t="n">
+        <v>142.9592566118656</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>44233</v>
+      </c>
+      <c r="B158" t="n">
+        <v>1</v>
+      </c>
+      <c r="C158" t="n">
+        <v>5</v>
+      </c>
+      <c r="D158" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+      <c r="C159" t="n">
+        <v>5</v>
+      </c>
+      <c r="D159" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B160" t="n">
+        <v>2</v>
+      </c>
+      <c r="C160" t="n">
+        <v>4</v>
+      </c>
+      <c r="D160" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
+      <c r="C161" t="n">
+        <v>3</v>
+      </c>
+      <c r="D161" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>44237</v>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
+      <c r="C162" t="n">
+        <v>2</v>
+      </c>
+      <c r="D162" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+      <c r="C163" t="n">
+        <v>2</v>
+      </c>
+      <c r="D163" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>44239</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
+      <c r="C164" t="n">
+        <v>2</v>
+      </c>
+      <c r="D164" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+      <c r="C165" t="n">
+        <v>3</v>
+      </c>
+      <c r="D165" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>44241</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
+      <c r="C166" t="n">
+        <v>3</v>
+      </c>
+      <c r="D166" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>44242</v>
+      </c>
+      <c r="B167" t="n">
+        <v>2</v>
+      </c>
+      <c r="C167" t="n">
+        <v>3</v>
+      </c>
+      <c r="D167" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B168" t="n">
+        <v>1</v>
+      </c>
+      <c r="C168" t="n">
+        <v>5</v>
+      </c>
+      <c r="D168" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>44244</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+      <c r="C169" t="n">
+        <v>7</v>
+      </c>
+      <c r="D169" t="n">
+        <v>166.7857993805099</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B170" t="n">
+        <v>0</v>
+      </c>
+      <c r="C170" t="n">
+        <v>11</v>
+      </c>
+      <c r="D170" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>44246</v>
+      </c>
+      <c r="B171" t="n">
+        <v>2</v>
+      </c>
+      <c r="C171" t="n">
+        <v>10</v>
+      </c>
+      <c r="D171" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B172" t="n">
+        <v>2</v>
+      </c>
+      <c r="C172" t="n">
+        <v>10</v>
+      </c>
+      <c r="D172" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B173" t="n">
+        <v>4</v>
+      </c>
+      <c r="C173" t="n">
+        <v>10</v>
+      </c>
+      <c r="D173" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B174" t="n">
+        <v>1</v>
+      </c>
+      <c r="C174" t="n">
+        <v>11</v>
+      </c>
+      <c r="D174" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>44250</v>
+      </c>
+      <c r="B175" t="n">
+        <v>1</v>
+      </c>
+      <c r="C175" t="n">
+        <v>12</v>
+      </c>
+      <c r="D175" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0</v>
+      </c>
+      <c r="C176" t="n">
+        <v>10</v>
+      </c>
+      <c r="D176" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B177" t="n">
+        <v>1</v>
+      </c>
+      <c r="C177" t="n">
+        <v>8</v>
+      </c>
+      <c r="D177" t="n">
+        <v>190.6123421491542</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B178" t="n">
+        <v>3</v>
+      </c>
+      <c r="C178" t="n">
+        <v>12</v>
+      </c>
+      <c r="D178" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0</v>
+      </c>
+      <c r="C179" t="n">
+        <v>12</v>
+      </c>
+      <c r="D179" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B180" t="n">
+        <v>2</v>
+      </c>
+      <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B181" t="n">
+        <v>5</v>
+      </c>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
         <v>44257</v>
       </c>
-      <c r="B145" t="n">
-        <v>1</v>
-      </c>
-      <c r="C145" t="inlineStr"/>
-      <c r="D145" t="inlineStr"/>
+      <c r="B182" t="n">
+        <v>1</v>
+      </c>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
finestra incidenza 7gg centrata su ultimo g
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -426,12 +426,8 @@
       <c r="B5" t="n">
         <v>0</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -440,12 +436,8 @@
       <c r="B6" t="n">
         <v>0</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -454,12 +446,8 @@
       <c r="B7" t="n">
         <v>0</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -511,10 +499,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -525,10 +513,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -539,10 +527,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -553,10 +541,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>47.65308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="15">
@@ -567,10 +555,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>47.65308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="16">
@@ -581,10 +569,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>47.65308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="17">
@@ -609,10 +597,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>23.82654276864427</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="19">
@@ -623,10 +611,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>23.82654276864427</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="20">
@@ -637,10 +625,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>23.82654276864427</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="21">
@@ -651,10 +639,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="22">
@@ -665,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="23">
@@ -679,10 +667,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="24">
@@ -931,10 +919,10 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -945,10 +933,10 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>23.82654276864427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -959,10 +947,10 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>47.65308553728854</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -973,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>47.65308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="45">
@@ -987,10 +975,10 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>47.65308553728854</v>
+        <v>23.82654276864427</v>
       </c>
     </row>
     <row r="46">
@@ -1001,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>95.30617107457708</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="47">
@@ -1015,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>119.1327138432213</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="48">
@@ -1029,10 +1017,10 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>95.30617107457708</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="49">
@@ -1043,10 +1031,10 @@
         <v>2</v>
       </c>
       <c r="C49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D49" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="50">
@@ -1057,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="51">
@@ -1085,10 +1073,10 @@
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D52" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="53">
@@ -1099,10 +1087,10 @@
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D53" t="n">
-        <v>71.47962830593281</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="54">
@@ -1113,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D54" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="55">
@@ -1127,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D55" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="56">
@@ -1141,10 +1129,10 @@
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" t="n">
-        <v>47.65308553728854</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="57">
@@ -1155,10 +1143,10 @@
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="58">
@@ -1169,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D58" t="n">
-        <v>119.1327138432213</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="59">
@@ -1183,10 +1171,10 @@
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>142.9592566118656</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="60">
@@ -1197,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D60" t="n">
-        <v>142.9592566118656</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="61">
@@ -1211,10 +1199,10 @@
         <v>2</v>
       </c>
       <c r="C61" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D61" t="n">
-        <v>166.7857993805099</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="62">
@@ -1225,10 +1213,10 @@
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D62" t="n">
-        <v>285.9185132237312</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="63">
@@ -1239,10 +1227,10 @@
         <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>357.398141529664</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="64">
@@ -1253,10 +1241,10 @@
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D64" t="n">
-        <v>405.0512270669526</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="65">
@@ -1267,10 +1255,10 @@
         <v>5</v>
       </c>
       <c r="C65" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D65" t="n">
-        <v>381.2246842983083</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="66">
@@ -1281,10 +1269,10 @@
         <v>4</v>
       </c>
       <c r="C66" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D66" t="n">
-        <v>428.8777698355968</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="67">
@@ -1295,10 +1283,10 @@
         <v>3</v>
       </c>
       <c r="C67" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D67" t="n">
-        <v>548.0104836788182</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="68">
@@ -1309,10 +1297,10 @@
         <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D68" t="n">
-        <v>643.3166547533953</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="69">
@@ -1323,10 +1311,10 @@
         <v>3</v>
       </c>
       <c r="C69" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D69" t="n">
-        <v>690.9697402906838</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="70">
@@ -1337,10 +1325,10 @@
         <v>6</v>
       </c>
       <c r="C70" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D70" t="n">
-        <v>643.3166547533953</v>
+        <v>548.0104836788182</v>
       </c>
     </row>
     <row r="71">
@@ -1351,10 +1339,10 @@
         <v>5</v>
       </c>
       <c r="C71" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D71" t="n">
-        <v>833.9289969025494</v>
+        <v>643.3166547533953</v>
       </c>
     </row>
     <row r="72">
@@ -1365,10 +1353,10 @@
         <v>7</v>
       </c>
       <c r="C72" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D72" t="n">
-        <v>833.9289969025494</v>
+        <v>690.9697402906838</v>
       </c>
     </row>
     <row r="73">
@@ -1379,10 +1367,10 @@
         <v>2</v>
       </c>
       <c r="C73" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D73" t="n">
-        <v>833.9289969025494</v>
+        <v>643.3166547533953</v>
       </c>
     </row>
     <row r="74">
@@ -1393,10 +1381,10 @@
         <v>11</v>
       </c>
       <c r="C74" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D74" t="n">
-        <v>810.1024541339052</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="75">
@@ -1407,10 +1395,10 @@
         <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D75" t="n">
-        <v>714.7962830593281</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="76">
@@ -1421,10 +1409,10 @@
         <v>3</v>
       </c>
       <c r="C76" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D76" t="n">
-        <v>595.6635692161067</v>
+        <v>833.9289969025494</v>
       </c>
     </row>
     <row r="77">
@@ -1435,10 +1423,10 @@
         <v>5</v>
       </c>
       <c r="C77" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D77" t="n">
-        <v>690.9697402906838</v>
+        <v>810.1024541339052</v>
       </c>
     </row>
     <row r="78">
@@ -1449,10 +1437,10 @@
         <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D78" t="n">
-        <v>428.8777698355968</v>
+        <v>714.7962830593281</v>
       </c>
     </row>
     <row r="79">
@@ -1463,10 +1451,10 @@
         <v>2</v>
       </c>
       <c r="C79" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D79" t="n">
-        <v>476.5308553728854</v>
+        <v>595.6635692161067</v>
       </c>
     </row>
     <row r="80">
@@ -1477,10 +1465,10 @@
         <v>6</v>
       </c>
       <c r="C80" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D80" t="n">
-        <v>500.3573981415297</v>
+        <v>690.9697402906838</v>
       </c>
     </row>
     <row r="81">
@@ -1491,10 +1479,10 @@
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D81" t="n">
-        <v>452.7043126042411</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="82">
@@ -1519,10 +1507,10 @@
         <v>4</v>
       </c>
       <c r="C83" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D83" t="n">
-        <v>524.183940910174</v>
+        <v>500.3573981415297</v>
       </c>
     </row>
     <row r="84">
@@ -1533,10 +1521,10 @@
         <v>3</v>
       </c>
       <c r="C84" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D84" t="n">
-        <v>428.8777698355968</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="85">
@@ -1561,10 +1549,10 @@
         <v>4</v>
       </c>
       <c r="C86" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D86" t="n">
-        <v>476.5308553728854</v>
+        <v>524.183940910174</v>
       </c>
     </row>
     <row r="87">
@@ -1589,10 +1577,10 @@
         <v>2</v>
       </c>
       <c r="C88" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D88" t="n">
-        <v>381.2246842983083</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="89">
@@ -1603,10 +1591,10 @@
         <v>3</v>
       </c>
       <c r="C89" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D89" t="n">
-        <v>357.398141529664</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="90">
@@ -1617,10 +1605,10 @@
         <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D90" t="n">
-        <v>285.9185132237312</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="91">
@@ -1631,10 +1619,10 @@
         <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D91" t="n">
-        <v>238.2654276864427</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="92">
@@ -1645,10 +1633,10 @@
         <v>1</v>
       </c>
       <c r="C92" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D92" t="n">
-        <v>214.4388849177984</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="93">
@@ -1659,10 +1647,10 @@
         <v>1</v>
       </c>
       <c r="C93" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D93" t="n">
-        <v>166.7857993805099</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="94">
@@ -1673,10 +1661,10 @@
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D94" t="n">
-        <v>262.091970455087</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="95">
@@ -1687,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D95" t="n">
-        <v>238.2654276864427</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="96">
@@ -1701,10 +1689,10 @@
         <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D96" t="n">
-        <v>309.7450559923755</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="97">
@@ -1715,10 +1703,10 @@
         <v>6</v>
       </c>
       <c r="C97" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D97" t="n">
-        <v>309.7450559923755</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="98">
@@ -1729,10 +1717,10 @@
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D98" t="n">
-        <v>333.5715987610197</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="99">
@@ -1743,10 +1731,10 @@
         <v>4</v>
       </c>
       <c r="C99" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D99" t="n">
-        <v>333.5715987610197</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="100">
@@ -1757,10 +1745,10 @@
         <v>1</v>
       </c>
       <c r="C100" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D100" t="n">
-        <v>357.398141529664</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="101">
@@ -1785,10 +1773,10 @@
         <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D102" t="n">
-        <v>452.7043126042411</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="103">
@@ -1799,10 +1787,10 @@
         <v>2</v>
       </c>
       <c r="C103" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D103" t="n">
-        <v>381.2246842983083</v>
+        <v>357.398141529664</v>
       </c>
     </row>
     <row r="104">
@@ -1813,10 +1801,10 @@
         <v>5</v>
       </c>
       <c r="C104" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D104" t="n">
-        <v>428.8777698355968</v>
+        <v>333.5715987610197</v>
       </c>
     </row>
     <row r="105">
@@ -1827,10 +1815,10 @@
         <v>5</v>
       </c>
       <c r="C105" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D105" t="n">
-        <v>405.0512270669526</v>
+        <v>452.7043126042411</v>
       </c>
     </row>
     <row r="106">
@@ -1841,10 +1829,10 @@
         <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D106" t="n">
-        <v>476.5308553728854</v>
+        <v>381.2246842983083</v>
       </c>
     </row>
     <row r="107">
@@ -1855,10 +1843,10 @@
         <v>3</v>
       </c>
       <c r="C107" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D107" t="n">
-        <v>476.5308553728854</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="108">
@@ -1869,10 +1857,10 @@
         <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D108" t="n">
-        <v>428.8777698355968</v>
+        <v>405.0512270669526</v>
       </c>
     </row>
     <row r="109">
@@ -1883,10 +1871,10 @@
         <v>4</v>
       </c>
       <c r="C109" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D109" t="n">
-        <v>309.7450559923755</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="110">
@@ -1897,10 +1885,10 @@
         <v>2</v>
       </c>
       <c r="C110" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D110" t="n">
-        <v>285.9185132237312</v>
+        <v>476.5308553728854</v>
       </c>
     </row>
     <row r="111">
@@ -1911,10 +1899,10 @@
         <v>3</v>
       </c>
       <c r="C111" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D111" t="n">
-        <v>214.4388849177984</v>
+        <v>428.8777698355968</v>
       </c>
     </row>
     <row r="112">
@@ -1925,10 +1913,10 @@
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D112" t="n">
-        <v>214.4388849177984</v>
+        <v>309.7450559923755</v>
       </c>
     </row>
     <row r="113">
@@ -1939,10 +1927,10 @@
         <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D113" t="n">
-        <v>119.1327138432213</v>
+        <v>285.9185132237312</v>
       </c>
     </row>
     <row r="114">
@@ -1953,10 +1941,10 @@
         <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D114" t="n">
-        <v>119.1327138432213</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="115">
@@ -1967,10 +1955,10 @@
         <v>0</v>
       </c>
       <c r="C115" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D115" t="n">
-        <v>71.47962830593281</v>
+        <v>214.4388849177984</v>
       </c>
     </row>
     <row r="116">
@@ -1981,10 +1969,10 @@
         <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D116" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="117">
@@ -1995,10 +1983,10 @@
         <v>2</v>
       </c>
       <c r="C117" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D117" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="118">
@@ -2009,10 +1997,10 @@
         <v>1</v>
       </c>
       <c r="C118" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D118" t="n">
-        <v>142.9592566118656</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="119">
@@ -2023,10 +2011,10 @@
         <v>3</v>
       </c>
       <c r="C119" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D119" t="n">
-        <v>166.7857993805099</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="120">
@@ -2037,10 +2025,10 @@
         <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D120" t="n">
-        <v>262.091970455087</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="121">
@@ -2051,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="C121" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D121" t="n">
-        <v>262.091970455087</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="122">
@@ -2065,10 +2053,10 @@
         <v>1</v>
       </c>
       <c r="C122" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D122" t="n">
-        <v>238.2654276864427</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="123">
@@ -2079,10 +2067,10 @@
         <v>4</v>
       </c>
       <c r="C123" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D123" t="n">
-        <v>190.6123421491542</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="124">
@@ -2093,10 +2081,10 @@
         <v>2</v>
       </c>
       <c r="C124" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D124" t="n">
-        <v>190.6123421491542</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="125">
@@ -2121,10 +2109,10 @@
         <v>1</v>
       </c>
       <c r="C126" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D126" t="n">
-        <v>238.2654276864427</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="127">
@@ -2135,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="C127" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D127" t="n">
-        <v>166.7857993805099</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="128">
@@ -2149,10 +2137,10 @@
         <v>2</v>
       </c>
       <c r="C128" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D128" t="n">
-        <v>119.1327138432213</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="129">
@@ -2163,10 +2151,10 @@
         <v>1</v>
       </c>
       <c r="C129" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D129" t="n">
-        <v>142.9592566118656</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="130">
@@ -2177,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="C130" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D130" t="n">
-        <v>142.9592566118656</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="131">
@@ -2191,10 +2179,10 @@
         <v>0</v>
       </c>
       <c r="C131" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D131" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="132">
@@ -2205,10 +2193,10 @@
         <v>1</v>
       </c>
       <c r="C132" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D132" t="n">
-        <v>119.1327138432213</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="133">
@@ -2219,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="C133" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D133" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="134">
@@ -2247,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="C135" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D135" t="n">
-        <v>142.9592566118656</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="136">
@@ -2261,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="C136" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D136" t="n">
-        <v>142.9592566118656</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="137">
@@ -2289,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="C138" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D138" t="n">
-        <v>190.6123421491542</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="139">
@@ -2303,10 +2291,10 @@
         <v>1</v>
       </c>
       <c r="C139" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D139" t="n">
-        <v>166.7857993805099</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="140">
@@ -2317,10 +2305,10 @@
         <v>1</v>
       </c>
       <c r="C140" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D140" t="n">
-        <v>166.7857993805099</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="141">
@@ -2331,10 +2319,10 @@
         <v>2</v>
       </c>
       <c r="C141" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D141" t="n">
-        <v>95.30617107457708</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="142">
@@ -2345,10 +2333,10 @@
         <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D142" t="n">
-        <v>142.9592566118656</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="143">
@@ -2359,10 +2347,10 @@
         <v>0</v>
       </c>
       <c r="C143" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D143" t="n">
-        <v>119.1327138432213</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="144">
@@ -2373,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="C144" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D144" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="145">
@@ -2387,10 +2375,10 @@
         <v>2</v>
       </c>
       <c r="C145" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D145" t="n">
-        <v>71.47962830593281</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="146">
@@ -2401,10 +2389,10 @@
         <v>0</v>
       </c>
       <c r="C146" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D146" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="147">
@@ -2415,10 +2403,10 @@
         <v>1</v>
       </c>
       <c r="C147" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D147" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="148">
@@ -2429,10 +2417,10 @@
         <v>0</v>
       </c>
       <c r="C148" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D148" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="149">
@@ -2457,10 +2445,10 @@
         <v>0</v>
       </c>
       <c r="C150" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D150" t="n">
-        <v>95.30617107457708</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="151">
@@ -2471,10 +2459,10 @@
         <v>2</v>
       </c>
       <c r="C151" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D151" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="152">
@@ -2485,10 +2473,10 @@
         <v>0</v>
       </c>
       <c r="C152" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D152" t="n">
-        <v>95.30617107457708</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="153">
@@ -2513,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="C154" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D154" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="155">
@@ -2541,10 +2529,10 @@
         <v>0</v>
       </c>
       <c r="C156" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D156" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="157">
@@ -2555,10 +2543,10 @@
         <v>1</v>
       </c>
       <c r="C157" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D157" t="n">
-        <v>95.30617107457708</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="158">
@@ -2569,10 +2557,10 @@
         <v>1</v>
       </c>
       <c r="C158" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D158" t="n">
-        <v>142.9592566118656</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="159">
@@ -2597,10 +2585,10 @@
         <v>0</v>
       </c>
       <c r="C160" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D160" t="n">
-        <v>119.1327138432213</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="161">
@@ -2611,10 +2599,10 @@
         <v>2</v>
       </c>
       <c r="C161" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D161" t="n">
-        <v>95.30617107457708</v>
+        <v>142.9592566118656</v>
       </c>
     </row>
     <row r="162">
@@ -2625,10 +2613,10 @@
         <v>0</v>
       </c>
       <c r="C162" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D162" t="n">
-        <v>71.47962830593281</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="163">
@@ -2639,10 +2627,10 @@
         <v>0</v>
       </c>
       <c r="C163" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D163" t="n">
-        <v>47.65308553728854</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="164">
@@ -2653,10 +2641,10 @@
         <v>0</v>
       </c>
       <c r="C164" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D164" t="n">
-        <v>47.65308553728854</v>
+        <v>95.30617107457708</v>
       </c>
     </row>
     <row r="165">
@@ -2667,10 +2655,10 @@
         <v>0</v>
       </c>
       <c r="C165" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D165" t="n">
-        <v>47.65308553728854</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="166">
@@ -2681,10 +2669,10 @@
         <v>0</v>
       </c>
       <c r="C166" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D166" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="167">
@@ -2695,10 +2683,10 @@
         <v>0</v>
       </c>
       <c r="C167" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D167" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="168">
@@ -2709,10 +2697,10 @@
         <v>2</v>
       </c>
       <c r="C168" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D168" t="n">
-        <v>71.47962830593281</v>
+        <v>47.65308553728854</v>
       </c>
     </row>
     <row r="169">
@@ -2723,10 +2711,10 @@
         <v>1</v>
       </c>
       <c r="C169" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D169" t="n">
-        <v>119.1327138432213</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="170">
@@ -2737,10 +2725,10 @@
         <v>0</v>
       </c>
       <c r="C170" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D170" t="n">
-        <v>166.7857993805099</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="171">
@@ -2751,10 +2739,10 @@
         <v>0</v>
       </c>
       <c r="C171" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D171" t="n">
-        <v>262.091970455087</v>
+        <v>71.47962830593281</v>
       </c>
     </row>
     <row r="172">
@@ -2765,10 +2753,10 @@
         <v>2</v>
       </c>
       <c r="C172" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D172" t="n">
-        <v>238.2654276864427</v>
+        <v>119.1327138432213</v>
       </c>
     </row>
     <row r="173">
@@ -2779,10 +2767,10 @@
         <v>2</v>
       </c>
       <c r="C173" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D173" t="n">
-        <v>238.2654276864427</v>
+        <v>166.7857993805099</v>
       </c>
     </row>
     <row r="174">
@@ -2793,10 +2781,10 @@
         <v>4</v>
       </c>
       <c r="C174" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D174" t="n">
-        <v>238.2654276864427</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="175">
@@ -2807,10 +2795,10 @@
         <v>1</v>
       </c>
       <c r="C175" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D175" t="n">
-        <v>262.091970455087</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="176">
@@ -2821,10 +2809,10 @@
         <v>1</v>
       </c>
       <c r="C176" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D176" t="n">
-        <v>285.9185132237312</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="177">
@@ -2849,10 +2837,10 @@
         <v>1</v>
       </c>
       <c r="C178" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D178" t="n">
-        <v>190.6123421491542</v>
+        <v>262.091970455087</v>
       </c>
     </row>
     <row r="179">
@@ -2877,10 +2865,10 @@
         <v>0</v>
       </c>
       <c r="C180" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D180" t="n">
-        <v>285.9185132237312</v>
+        <v>238.2654276864427</v>
       </c>
     </row>
     <row r="181">
@@ -2891,10 +2879,10 @@
         <v>2</v>
       </c>
       <c r="C181" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D181" t="n">
-        <v>285.9185132237312</v>
+        <v>190.6123421491542</v>
       </c>
     </row>
     <row r="182">
@@ -2904,8 +2892,12 @@
       <c r="B182" t="n">
         <v>5</v>
       </c>
-      <c r="C182" t="inlineStr"/>
-      <c r="D182" t="inlineStr"/>
+      <c r="C182" t="n">
+        <v>12</v>
+      </c>
+      <c r="D182" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
@@ -2914,8 +2906,12 @@
       <c r="B183" t="n">
         <v>1</v>
       </c>
-      <c r="C183" t="inlineStr"/>
-      <c r="D183" t="inlineStr"/>
+      <c r="C183" t="n">
+        <v>12</v>
+      </c>
+      <c r="D183" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
@@ -2924,8 +2920,12 @@
       <c r="B184" t="n">
         <v>0</v>
       </c>
-      <c r="C184" t="inlineStr"/>
-      <c r="D184" t="inlineStr"/>
+      <c r="C184" t="n">
+        <v>12</v>
+      </c>
+      <c r="D184" t="n">
+        <v>285.9185132237312</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
aggiornamenti 21 e 22 marzo
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3165,6 +3165,34 @@
         <v>285.9185132237312</v>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" s="2" t="n">
+        <v>44276</v>
+      </c>
+      <c r="B202" t="n">
+        <v>4</v>
+      </c>
+      <c r="C202" t="n">
+        <v>15</v>
+      </c>
+      <c r="D202" t="n">
+        <v>357.398141529664</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0</v>
+      </c>
+      <c r="C203" t="n">
+        <v>14</v>
+      </c>
+      <c r="D203" t="n">
+        <v>333.5715987610197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento 24 e 25 marzo 2021
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3207,6 +3207,34 @@
         <v>285.9185132237312</v>
       </c>
     </row>
+    <row r="205">
+      <c r="A205" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0</v>
+      </c>
+      <c r="C205" t="n">
+        <v>12</v>
+      </c>
+      <c r="D205" t="n">
+        <v>285.9185132237312</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0</v>
+      </c>
+      <c r="C206" t="n">
+        <v>5</v>
+      </c>
+      <c r="D206" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento 13 e 14 aprile
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D224"/>
+  <dimension ref="A1:D226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3487,6 +3487,34 @@
         <v>428.8777698355968</v>
       </c>
     </row>
+    <row r="225">
+      <c r="A225" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B225" t="n">
+        <v>2</v>
+      </c>
+      <c r="C225" t="n">
+        <v>20</v>
+      </c>
+      <c r="D225" t="n">
+        <v>476.5308553728854</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="2" t="n">
+        <v>44300</v>
+      </c>
+      <c r="B226" t="n">
+        <v>0</v>
+      </c>
+      <c r="C226" t="n">
+        <v>20</v>
+      </c>
+      <c r="D226" t="n">
+        <v>476.5308553728854</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento 15, 16, 17 marzo
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D226"/>
+  <dimension ref="A1:D229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3515,6 +3515,48 @@
         <v>476.5308553728854</v>
       </c>
     </row>
+    <row r="227">
+      <c r="A227" s="2" t="n">
+        <v>44301</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0</v>
+      </c>
+      <c r="C227" t="n">
+        <v>20</v>
+      </c>
+      <c r="D227" t="n">
+        <v>476.5308553728854</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B228" t="n">
+        <v>1</v>
+      </c>
+      <c r="C228" t="n">
+        <v>20</v>
+      </c>
+      <c r="D228" t="n">
+        <v>476.5308553728854</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="n">
+        <v>44303</v>
+      </c>
+      <c r="B229" t="n">
+        <v>1</v>
+      </c>
+      <c r="C229" t="n">
+        <v>18</v>
+      </c>
+      <c r="D229" t="n">
+        <v>428.8777698355968</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 21 marzo
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D229"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3557,6 +3557,62 @@
         <v>428.8777698355968</v>
       </c>
     </row>
+    <row r="230">
+      <c r="A230" s="2" t="n">
+        <v>44304</v>
+      </c>
+      <c r="B230" t="n">
+        <v>1</v>
+      </c>
+      <c r="C230" t="n">
+        <v>19</v>
+      </c>
+      <c r="D230" t="n">
+        <v>452.7043126042411</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="2" t="n">
+        <v>44305</v>
+      </c>
+      <c r="B231" t="n">
+        <v>0</v>
+      </c>
+      <c r="C231" t="n">
+        <v>5</v>
+      </c>
+      <c r="D231" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B232" t="n">
+        <v>0</v>
+      </c>
+      <c r="C232" t="n">
+        <v>3</v>
+      </c>
+      <c r="D232" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="2" t="n">
+        <v>44307</v>
+      </c>
+      <c r="B233" t="n">
+        <v>0</v>
+      </c>
+      <c r="C233" t="n">
+        <v>3</v>
+      </c>
+      <c r="D233" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino al 26/03
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3613,6 +3613,76 @@
         <v>71.47962830593281</v>
       </c>
     </row>
+    <row r="234">
+      <c r="A234" s="2" t="n">
+        <v>44308</v>
+      </c>
+      <c r="B234" t="n">
+        <v>1</v>
+      </c>
+      <c r="C234" t="n">
+        <v>4</v>
+      </c>
+      <c r="D234" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B235" t="n">
+        <v>2</v>
+      </c>
+      <c r="C235" t="n">
+        <v>5</v>
+      </c>
+      <c r="D235" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="2" t="n">
+        <v>44310</v>
+      </c>
+      <c r="B236" t="n">
+        <v>1</v>
+      </c>
+      <c r="C236" t="n">
+        <v>5</v>
+      </c>
+      <c r="D236" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="2" t="n">
+        <v>44311</v>
+      </c>
+      <c r="B237" t="n">
+        <v>6</v>
+      </c>
+      <c r="C237" t="n">
+        <v>10</v>
+      </c>
+      <c r="D237" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B238" t="n">
+        <v>0</v>
+      </c>
+      <c r="C238" t="n">
+        <v>10</v>
+      </c>
+      <c r="D238" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 02/05
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D238"/>
+  <dimension ref="A1:D244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3683,6 +3683,90 @@
         <v>238.2654276864427</v>
       </c>
     </row>
+    <row r="239">
+      <c r="A239" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B239" t="n">
+        <v>0</v>
+      </c>
+      <c r="C239" t="n">
+        <v>10</v>
+      </c>
+      <c r="D239" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B240" t="n">
+        <v>0</v>
+      </c>
+      <c r="C240" t="n">
+        <v>10</v>
+      </c>
+      <c r="D240" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B241" t="n">
+        <v>1</v>
+      </c>
+      <c r="C241" t="n">
+        <v>10</v>
+      </c>
+      <c r="D241" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B242" t="n">
+        <v>2</v>
+      </c>
+      <c r="C242" t="n">
+        <v>10</v>
+      </c>
+      <c r="D242" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B243" t="n">
+        <v>0</v>
+      </c>
+      <c r="C243" t="n">
+        <v>9</v>
+      </c>
+      <c r="D243" t="n">
+        <v>214.4388849177984</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="2" t="n">
+        <v>44318</v>
+      </c>
+      <c r="B244" t="n">
+        <v>0</v>
+      </c>
+      <c r="C244" t="n">
+        <v>3</v>
+      </c>
+      <c r="D244" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 6/03
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D244"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3767,6 +3767,48 @@
         <v>71.47962830593281</v>
       </c>
     </row>
+    <row r="245">
+      <c r="A245" s="2" t="n">
+        <v>44319</v>
+      </c>
+      <c r="B245" t="n">
+        <v>1</v>
+      </c>
+      <c r="C245" t="n">
+        <v>4</v>
+      </c>
+      <c r="D245" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2" t="n">
+        <v>44320</v>
+      </c>
+      <c r="B246" t="n">
+        <v>0</v>
+      </c>
+      <c r="C246" t="n">
+        <v>4</v>
+      </c>
+      <c r="D246" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B247" t="n">
+        <v>0</v>
+      </c>
+      <c r="C247" t="n">
+        <v>4</v>
+      </c>
+      <c r="D247" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 7/03+
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:D249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3809,6 +3809,34 @@
         <v>95.30617107457708</v>
       </c>
     </row>
+    <row r="248">
+      <c r="A248" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B248" t="n">
+        <v>0</v>
+      </c>
+      <c r="C248" t="n">
+        <v>3</v>
+      </c>
+      <c r="D248" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="2" t="n">
+        <v>44323</v>
+      </c>
+      <c r="B249" t="n">
+        <v>3</v>
+      </c>
+      <c r="C249" t="n">
+        <v>4</v>
+      </c>
+      <c r="D249" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 9/05
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D249"/>
+  <dimension ref="A1:D251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3837,6 +3837,34 @@
         <v>95.30617107457708</v>
       </c>
     </row>
+    <row r="250">
+      <c r="A250" s="2" t="n">
+        <v>44324</v>
+      </c>
+      <c r="B250" t="n">
+        <v>2</v>
+      </c>
+      <c r="C250" t="n">
+        <v>6</v>
+      </c>
+      <c r="D250" t="n">
+        <v>142.9592566118656</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="2" t="n">
+        <v>44325</v>
+      </c>
+      <c r="B251" t="n">
+        <v>0</v>
+      </c>
+      <c r="C251" t="n">
+        <v>6</v>
+      </c>
+      <c r="D251" t="n">
+        <v>142.9592566118656</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 13/03
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D251"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3865,6 +3865,62 @@
         <v>142.9592566118656</v>
       </c>
     </row>
+    <row r="252">
+      <c r="A252" s="2" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B252" t="n">
+        <v>0</v>
+      </c>
+      <c r="C252" t="n">
+        <v>5</v>
+      </c>
+      <c r="D252" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B253" t="n">
+        <v>0</v>
+      </c>
+      <c r="C253" t="n">
+        <v>5</v>
+      </c>
+      <c r="D253" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="2" t="n">
+        <v>44328</v>
+      </c>
+      <c r="B254" t="n">
+        <v>0</v>
+      </c>
+      <c r="C254" t="n">
+        <v>5</v>
+      </c>
+      <c r="D254" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="2" t="n">
+        <v>44329</v>
+      </c>
+      <c r="B255" t="n">
+        <v>0</v>
+      </c>
+      <c r="C255" t="n">
+        <v>5</v>
+      </c>
+      <c r="D255" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 27/05
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D255"/>
+  <dimension ref="A1:D269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3921,6 +3921,202 @@
         <v>119.1327138432213</v>
       </c>
     </row>
+    <row r="256">
+      <c r="A256" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B256" t="n">
+        <v>0</v>
+      </c>
+      <c r="C256" t="n">
+        <v>2</v>
+      </c>
+      <c r="D256" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="2" t="n">
+        <v>44331</v>
+      </c>
+      <c r="B257" t="n">
+        <v>1</v>
+      </c>
+      <c r="C257" t="n">
+        <v>1</v>
+      </c>
+      <c r="D257" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="2" t="n">
+        <v>44332</v>
+      </c>
+      <c r="B258" t="n">
+        <v>0</v>
+      </c>
+      <c r="C258" t="n">
+        <v>1</v>
+      </c>
+      <c r="D258" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B259" t="n">
+        <v>0</v>
+      </c>
+      <c r="C259" t="n">
+        <v>1</v>
+      </c>
+      <c r="D259" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B260" t="n">
+        <v>0</v>
+      </c>
+      <c r="C260" t="n">
+        <v>1</v>
+      </c>
+      <c r="D260" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B261" t="n">
+        <v>0</v>
+      </c>
+      <c r="C261" t="n">
+        <v>1</v>
+      </c>
+      <c r="D261" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B262" t="n">
+        <v>0</v>
+      </c>
+      <c r="C262" t="n">
+        <v>1</v>
+      </c>
+      <c r="D262" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B263" t="n">
+        <v>0</v>
+      </c>
+      <c r="C263" t="n">
+        <v>1</v>
+      </c>
+      <c r="D263" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="B264" t="n">
+        <v>0</v>
+      </c>
+      <c r="C264" t="n">
+        <v>0</v>
+      </c>
+      <c r="D264" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="2" t="n">
+        <v>44339</v>
+      </c>
+      <c r="B265" t="n">
+        <v>0</v>
+      </c>
+      <c r="C265" t="n">
+        <v>0</v>
+      </c>
+      <c r="D265" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B266" t="n">
+        <v>0</v>
+      </c>
+      <c r="C266" t="n">
+        <v>0</v>
+      </c>
+      <c r="D266" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B267" t="n">
+        <v>0</v>
+      </c>
+      <c r="C267" t="n">
+        <v>0</v>
+      </c>
+      <c r="D267" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B268" t="n">
+        <v>0</v>
+      </c>
+      <c r="C268" t="n">
+        <v>0</v>
+      </c>
+      <c r="D268" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B269" t="n">
+        <v>0</v>
+      </c>
+      <c r="C269" t="n">
+        <v>0</v>
+      </c>
+      <c r="D269" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 28/06 incluso
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D269"/>
+  <dimension ref="A1:D301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4117,6 +4117,454 @@
         <v>0</v>
       </c>
     </row>
+    <row r="270">
+      <c r="A270" s="2" t="n">
+        <v>44344</v>
+      </c>
+      <c r="B270" t="n">
+        <v>0</v>
+      </c>
+      <c r="C270" t="n">
+        <v>0</v>
+      </c>
+      <c r="D270" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="2" t="n">
+        <v>44345</v>
+      </c>
+      <c r="B271" t="n">
+        <v>0</v>
+      </c>
+      <c r="C271" t="n">
+        <v>0</v>
+      </c>
+      <c r="D271" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="2" t="n">
+        <v>44346</v>
+      </c>
+      <c r="B272" t="n">
+        <v>0</v>
+      </c>
+      <c r="C272" t="n">
+        <v>0</v>
+      </c>
+      <c r="D272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B273" t="n">
+        <v>1</v>
+      </c>
+      <c r="C273" t="n">
+        <v>1</v>
+      </c>
+      <c r="D273" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B274" t="n">
+        <v>0</v>
+      </c>
+      <c r="C274" t="n">
+        <v>1</v>
+      </c>
+      <c r="D274" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B275" t="n">
+        <v>0</v>
+      </c>
+      <c r="C275" t="n">
+        <v>1</v>
+      </c>
+      <c r="D275" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B276" t="n">
+        <v>1</v>
+      </c>
+      <c r="C276" t="n">
+        <v>2</v>
+      </c>
+      <c r="D276" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="2" t="n">
+        <v>44351</v>
+      </c>
+      <c r="B277" t="n">
+        <v>0</v>
+      </c>
+      <c r="C277" t="n">
+        <v>2</v>
+      </c>
+      <c r="D277" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="2" t="n">
+        <v>44352</v>
+      </c>
+      <c r="B278" t="n">
+        <v>0</v>
+      </c>
+      <c r="C278" t="n">
+        <v>2</v>
+      </c>
+      <c r="D278" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="2" t="n">
+        <v>44353</v>
+      </c>
+      <c r="B279" t="n">
+        <v>1</v>
+      </c>
+      <c r="C279" t="n">
+        <v>3</v>
+      </c>
+      <c r="D279" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B280" t="n">
+        <v>0</v>
+      </c>
+      <c r="C280" t="n">
+        <v>2</v>
+      </c>
+      <c r="D280" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B281" t="n">
+        <v>0</v>
+      </c>
+      <c r="C281" t="n">
+        <v>2</v>
+      </c>
+      <c r="D281" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B282" t="n">
+        <v>0</v>
+      </c>
+      <c r="C282" t="n">
+        <v>2</v>
+      </c>
+      <c r="D282" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="2" t="n">
+        <v>44357</v>
+      </c>
+      <c r="B283" t="n">
+        <v>0</v>
+      </c>
+      <c r="C283" t="n">
+        <v>1</v>
+      </c>
+      <c r="D283" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="2" t="n">
+        <v>44358</v>
+      </c>
+      <c r="B284" t="n">
+        <v>0</v>
+      </c>
+      <c r="C284" t="n">
+        <v>1</v>
+      </c>
+      <c r="D284" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="2" t="n">
+        <v>44359</v>
+      </c>
+      <c r="B285" t="n">
+        <v>0</v>
+      </c>
+      <c r="C285" t="n">
+        <v>1</v>
+      </c>
+      <c r="D285" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="2" t="n">
+        <v>44360</v>
+      </c>
+      <c r="B286" t="n">
+        <v>0</v>
+      </c>
+      <c r="C286" t="n">
+        <v>0</v>
+      </c>
+      <c r="D286" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B287" t="n">
+        <v>0</v>
+      </c>
+      <c r="C287" t="n">
+        <v>0</v>
+      </c>
+      <c r="D287" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B288" t="n">
+        <v>0</v>
+      </c>
+      <c r="C288" t="n">
+        <v>0</v>
+      </c>
+      <c r="D288" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B289" t="n">
+        <v>0</v>
+      </c>
+      <c r="C289" t="n">
+        <v>0</v>
+      </c>
+      <c r="D289" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="2" t="n">
+        <v>44364</v>
+      </c>
+      <c r="B290" t="n">
+        <v>0</v>
+      </c>
+      <c r="C290" t="n">
+        <v>0</v>
+      </c>
+      <c r="D290" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B291" t="n">
+        <v>0</v>
+      </c>
+      <c r="C291" t="n">
+        <v>0</v>
+      </c>
+      <c r="D291" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="2" t="n">
+        <v>44366</v>
+      </c>
+      <c r="B292" t="n">
+        <v>0</v>
+      </c>
+      <c r="C292" t="n">
+        <v>0</v>
+      </c>
+      <c r="D292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="2" t="n">
+        <v>44367</v>
+      </c>
+      <c r="B293" t="n">
+        <v>0</v>
+      </c>
+      <c r="C293" t="n">
+        <v>0</v>
+      </c>
+      <c r="D293" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B294" t="n">
+        <v>0</v>
+      </c>
+      <c r="C294" t="n">
+        <v>0</v>
+      </c>
+      <c r="D294" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B295" t="n">
+        <v>0</v>
+      </c>
+      <c r="C295" t="n">
+        <v>0</v>
+      </c>
+      <c r="D295" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="2" t="n">
+        <v>44370</v>
+      </c>
+      <c r="B296" t="n">
+        <v>0</v>
+      </c>
+      <c r="C296" t="n">
+        <v>0</v>
+      </c>
+      <c r="D296" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="2" t="n">
+        <v>44371</v>
+      </c>
+      <c r="B297" t="n">
+        <v>0</v>
+      </c>
+      <c r="C297" t="n">
+        <v>0</v>
+      </c>
+      <c r="D297" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="2" t="n">
+        <v>44372</v>
+      </c>
+      <c r="B298" t="n">
+        <v>0</v>
+      </c>
+      <c r="C298" t="n">
+        <v>0</v>
+      </c>
+      <c r="D298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B299" t="n">
+        <v>0</v>
+      </c>
+      <c r="C299" t="n">
+        <v>0</v>
+      </c>
+      <c r="D299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="2" t="n">
+        <v>44374</v>
+      </c>
+      <c r="B300" t="n">
+        <v>0</v>
+      </c>
+      <c r="C300" t="n">
+        <v>0</v>
+      </c>
+      <c r="D300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="2" t="n">
+        <v>44375</v>
+      </c>
+      <c r="B301" t="n">
+        <v>0</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0</v>
+      </c>
+      <c r="D301" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 28 luglio
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D301"/>
+  <dimension ref="A1:D328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4565,6 +4565,384 @@
         <v>0</v>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" s="2" t="n">
+        <v>44376</v>
+      </c>
+      <c r="B302" t="n">
+        <v>0</v>
+      </c>
+      <c r="C302" t="n">
+        <v>0</v>
+      </c>
+      <c r="D302" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="2" t="n">
+        <v>44377</v>
+      </c>
+      <c r="B303" t="n">
+        <v>0</v>
+      </c>
+      <c r="C303" t="n">
+        <v>0</v>
+      </c>
+      <c r="D303" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="2" t="n">
+        <v>44378</v>
+      </c>
+      <c r="B304" t="n">
+        <v>0</v>
+      </c>
+      <c r="C304" t="n">
+        <v>0</v>
+      </c>
+      <c r="D304" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="2" t="n">
+        <v>44379</v>
+      </c>
+      <c r="B305" t="n">
+        <v>0</v>
+      </c>
+      <c r="C305" t="n">
+        <v>0</v>
+      </c>
+      <c r="D305" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="2" t="n">
+        <v>44380</v>
+      </c>
+      <c r="B306" t="n">
+        <v>0</v>
+      </c>
+      <c r="C306" t="n">
+        <v>0</v>
+      </c>
+      <c r="D306" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="B307" t="n">
+        <v>0</v>
+      </c>
+      <c r="C307" t="n">
+        <v>0</v>
+      </c>
+      <c r="D307" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="2" t="n">
+        <v>44382</v>
+      </c>
+      <c r="B308" t="n">
+        <v>0</v>
+      </c>
+      <c r="C308" t="n">
+        <v>0</v>
+      </c>
+      <c r="D308" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="2" t="n">
+        <v>44383</v>
+      </c>
+      <c r="B309" t="n">
+        <v>0</v>
+      </c>
+      <c r="C309" t="n">
+        <v>0</v>
+      </c>
+      <c r="D309" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B310" t="n">
+        <v>0</v>
+      </c>
+      <c r="C310" t="n">
+        <v>0</v>
+      </c>
+      <c r="D310" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B311" t="n">
+        <v>0</v>
+      </c>
+      <c r="C311" t="n">
+        <v>0</v>
+      </c>
+      <c r="D311" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="2" t="n">
+        <v>44386</v>
+      </c>
+      <c r="B312" t="n">
+        <v>0</v>
+      </c>
+      <c r="C312" t="n">
+        <v>0</v>
+      </c>
+      <c r="D312" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="2" t="n">
+        <v>44387</v>
+      </c>
+      <c r="B313" t="n">
+        <v>0</v>
+      </c>
+      <c r="C313" t="n">
+        <v>0</v>
+      </c>
+      <c r="D313" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="2" t="n">
+        <v>44388</v>
+      </c>
+      <c r="B314" t="n">
+        <v>0</v>
+      </c>
+      <c r="C314" t="n">
+        <v>0</v>
+      </c>
+      <c r="D314" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="2" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B315" t="n">
+        <v>0</v>
+      </c>
+      <c r="C315" t="n">
+        <v>0</v>
+      </c>
+      <c r="D315" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="2" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B316" t="n">
+        <v>1</v>
+      </c>
+      <c r="C316" t="n">
+        <v>1</v>
+      </c>
+      <c r="D316" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="2" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B317" t="n">
+        <v>1</v>
+      </c>
+      <c r="C317" t="n">
+        <v>2</v>
+      </c>
+      <c r="D317" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="2" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B318" t="n">
+        <v>1</v>
+      </c>
+      <c r="C318" t="n">
+        <v>3</v>
+      </c>
+      <c r="D318" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="2" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B319" t="n">
+        <v>1</v>
+      </c>
+      <c r="C319" t="n">
+        <v>4</v>
+      </c>
+      <c r="D319" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="2" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B320" t="n">
+        <v>0</v>
+      </c>
+      <c r="C320" t="n">
+        <v>4</v>
+      </c>
+      <c r="D320" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="2" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B321" t="n">
+        <v>0</v>
+      </c>
+      <c r="C321" t="n">
+        <v>4</v>
+      </c>
+      <c r="D321" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="2" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B322" t="n">
+        <v>0</v>
+      </c>
+      <c r="C322" t="n">
+        <v>4</v>
+      </c>
+      <c r="D322" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="2" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B323" t="n">
+        <v>0</v>
+      </c>
+      <c r="C323" t="n">
+        <v>3</v>
+      </c>
+      <c r="D323" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="2" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B324" t="n">
+        <v>0</v>
+      </c>
+      <c r="C324" t="n">
+        <v>2</v>
+      </c>
+      <c r="D324" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="2" t="n">
+        <v>44399</v>
+      </c>
+      <c r="B325" t="n">
+        <v>0</v>
+      </c>
+      <c r="C325" t="n">
+        <v>1</v>
+      </c>
+      <c r="D325" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="2" t="n">
+        <v>44400</v>
+      </c>
+      <c r="B326" t="n">
+        <v>1</v>
+      </c>
+      <c r="C326" t="n">
+        <v>1</v>
+      </c>
+      <c r="D326" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="2" t="n">
+        <v>44401</v>
+      </c>
+      <c r="B327" t="n">
+        <v>2</v>
+      </c>
+      <c r="C327" t="n">
+        <v>3</v>
+      </c>
+      <c r="D327" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="2" t="n">
+        <v>44402</v>
+      </c>
+      <c r="B328" t="n">
+        <v>1</v>
+      </c>
+      <c r="C328" t="n">
+        <v>4</v>
+      </c>
+      <c r="D328" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 9 agosto 2021
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D328"/>
+  <dimension ref="A1:D343"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4943,6 +4943,216 @@
         <v>95.30617107457708</v>
       </c>
     </row>
+    <row r="329">
+      <c r="A329" s="2" t="n">
+        <v>44403</v>
+      </c>
+      <c r="B329" t="n">
+        <v>0</v>
+      </c>
+      <c r="C329" t="n">
+        <v>4</v>
+      </c>
+      <c r="D329" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="2" t="n">
+        <v>44404</v>
+      </c>
+      <c r="B330" t="n">
+        <v>0</v>
+      </c>
+      <c r="C330" t="n">
+        <v>4</v>
+      </c>
+      <c r="D330" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="2" t="n">
+        <v>44405</v>
+      </c>
+      <c r="B331" t="n">
+        <v>0</v>
+      </c>
+      <c r="C331" t="n">
+        <v>4</v>
+      </c>
+      <c r="D331" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="2" t="n">
+        <v>44406</v>
+      </c>
+      <c r="B332" t="n">
+        <v>0</v>
+      </c>
+      <c r="C332" t="n">
+        <v>4</v>
+      </c>
+      <c r="D332" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="2" t="n">
+        <v>44407</v>
+      </c>
+      <c r="B333" t="n">
+        <v>0</v>
+      </c>
+      <c r="C333" t="n">
+        <v>3</v>
+      </c>
+      <c r="D333" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="2" t="n">
+        <v>44408</v>
+      </c>
+      <c r="B334" t="n">
+        <v>0</v>
+      </c>
+      <c r="C334" t="n">
+        <v>1</v>
+      </c>
+      <c r="D334" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="2" t="n">
+        <v>44409</v>
+      </c>
+      <c r="B335" t="n">
+        <v>0</v>
+      </c>
+      <c r="C335" t="n">
+        <v>0</v>
+      </c>
+      <c r="D335" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="2" t="n">
+        <v>44410</v>
+      </c>
+      <c r="B336" t="n">
+        <v>2</v>
+      </c>
+      <c r="C336" t="n">
+        <v>2</v>
+      </c>
+      <c r="D336" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="2" t="n">
+        <v>44411</v>
+      </c>
+      <c r="B337" t="n">
+        <v>0</v>
+      </c>
+      <c r="C337" t="n">
+        <v>2</v>
+      </c>
+      <c r="D337" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="2" t="n">
+        <v>44412</v>
+      </c>
+      <c r="B338" t="n">
+        <v>0</v>
+      </c>
+      <c r="C338" t="n">
+        <v>2</v>
+      </c>
+      <c r="D338" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="2" t="n">
+        <v>44413</v>
+      </c>
+      <c r="B339" t="n">
+        <v>1</v>
+      </c>
+      <c r="C339" t="n">
+        <v>3</v>
+      </c>
+      <c r="D339" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="2" t="n">
+        <v>44414</v>
+      </c>
+      <c r="B340" t="n">
+        <v>1</v>
+      </c>
+      <c r="C340" t="n">
+        <v>4</v>
+      </c>
+      <c r="D340" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="2" t="n">
+        <v>44415</v>
+      </c>
+      <c r="B341" t="n">
+        <v>0</v>
+      </c>
+      <c r="C341" t="n">
+        <v>4</v>
+      </c>
+      <c r="D341" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="2" t="n">
+        <v>44416</v>
+      </c>
+      <c r="B342" t="n">
+        <v>1</v>
+      </c>
+      <c r="C342" t="n">
+        <v>5</v>
+      </c>
+      <c r="D342" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="2" t="n">
+        <v>44417</v>
+      </c>
+      <c r="B343" t="n">
+        <v>0</v>
+      </c>
+      <c r="C343" t="n">
+        <v>3</v>
+      </c>
+      <c r="D343" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento a l 23 agosto 2021
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D343"/>
+  <dimension ref="A1:D357"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5153,6 +5153,202 @@
         <v>71.47962830593281</v>
       </c>
     </row>
+    <row r="344">
+      <c r="A344" s="2" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B344" t="n">
+        <v>0</v>
+      </c>
+      <c r="C344" t="n">
+        <v>3</v>
+      </c>
+      <c r="D344" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="2" t="n">
+        <v>44419</v>
+      </c>
+      <c r="B345" t="n">
+        <v>0</v>
+      </c>
+      <c r="C345" t="n">
+        <v>3</v>
+      </c>
+      <c r="D345" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="2" t="n">
+        <v>44420</v>
+      </c>
+      <c r="B346" t="n">
+        <v>2</v>
+      </c>
+      <c r="C346" t="n">
+        <v>4</v>
+      </c>
+      <c r="D346" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="2" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B347" t="n">
+        <v>1</v>
+      </c>
+      <c r="C347" t="n">
+        <v>4</v>
+      </c>
+      <c r="D347" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="2" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B348" t="n">
+        <v>0</v>
+      </c>
+      <c r="C348" t="n">
+        <v>4</v>
+      </c>
+      <c r="D348" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="2" t="n">
+        <v>44423</v>
+      </c>
+      <c r="B349" t="n">
+        <v>0</v>
+      </c>
+      <c r="C349" t="n">
+        <v>3</v>
+      </c>
+      <c r="D349" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B350" t="n">
+        <v>1</v>
+      </c>
+      <c r="C350" t="n">
+        <v>4</v>
+      </c>
+      <c r="D350" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="2" t="n">
+        <v>44425</v>
+      </c>
+      <c r="B351" t="n">
+        <v>1</v>
+      </c>
+      <c r="C351" t="n">
+        <v>5</v>
+      </c>
+      <c r="D351" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="2" t="n">
+        <v>44426</v>
+      </c>
+      <c r="B352" t="n">
+        <v>0</v>
+      </c>
+      <c r="C352" t="n">
+        <v>5</v>
+      </c>
+      <c r="D352" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B353" t="n">
+        <v>0</v>
+      </c>
+      <c r="C353" t="n">
+        <v>3</v>
+      </c>
+      <c r="D353" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="2" t="n">
+        <v>44428</v>
+      </c>
+      <c r="B354" t="n">
+        <v>1</v>
+      </c>
+      <c r="C354" t="n">
+        <v>3</v>
+      </c>
+      <c r="D354" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="2" t="n">
+        <v>44429</v>
+      </c>
+      <c r="B355" t="n">
+        <v>0</v>
+      </c>
+      <c r="C355" t="n">
+        <v>3</v>
+      </c>
+      <c r="D355" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="2" t="n">
+        <v>44430</v>
+      </c>
+      <c r="B356" t="n">
+        <v>0</v>
+      </c>
+      <c r="C356" t="n">
+        <v>3</v>
+      </c>
+      <c r="D356" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="2" t="n">
+        <v>44431</v>
+      </c>
+      <c r="B357" t="n">
+        <v>1</v>
+      </c>
+      <c r="C357" t="n">
+        <v>3</v>
+      </c>
+      <c r="D357" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 1/09/2021
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D357"/>
+  <dimension ref="A1:D366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5349,6 +5349,132 @@
         <v>71.47962830593281</v>
       </c>
     </row>
+    <row r="358">
+      <c r="A358" s="2" t="n">
+        <v>44432</v>
+      </c>
+      <c r="B358" t="n">
+        <v>0</v>
+      </c>
+      <c r="C358" t="n">
+        <v>2</v>
+      </c>
+      <c r="D358" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="2" t="n">
+        <v>44433</v>
+      </c>
+      <c r="B359" t="n">
+        <v>0</v>
+      </c>
+      <c r="C359" t="n">
+        <v>2</v>
+      </c>
+      <c r="D359" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="2" t="n">
+        <v>44434</v>
+      </c>
+      <c r="B360" t="n">
+        <v>0</v>
+      </c>
+      <c r="C360" t="n">
+        <v>2</v>
+      </c>
+      <c r="D360" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="2" t="n">
+        <v>44435</v>
+      </c>
+      <c r="B361" t="n">
+        <v>1</v>
+      </c>
+      <c r="C361" t="n">
+        <v>2</v>
+      </c>
+      <c r="D361" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="2" t="n">
+        <v>44436</v>
+      </c>
+      <c r="B362" t="n">
+        <v>0</v>
+      </c>
+      <c r="C362" t="n">
+        <v>2</v>
+      </c>
+      <c r="D362" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="2" t="n">
+        <v>44437</v>
+      </c>
+      <c r="B363" t="n">
+        <v>0</v>
+      </c>
+      <c r="C363" t="n">
+        <v>2</v>
+      </c>
+      <c r="D363" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="2" t="n">
+        <v>44438</v>
+      </c>
+      <c r="B364" t="n">
+        <v>1</v>
+      </c>
+      <c r="C364" t="n">
+        <v>2</v>
+      </c>
+      <c r="D364" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="2" t="n">
+        <v>44439</v>
+      </c>
+      <c r="B365" t="n">
+        <v>0</v>
+      </c>
+      <c r="C365" t="n">
+        <v>2</v>
+      </c>
+      <c r="D365" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="2" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B366" t="n">
+        <v>0</v>
+      </c>
+      <c r="C366" t="n">
+        <v>2</v>
+      </c>
+      <c r="D366" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento a 9/09 compreso
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D366"/>
+  <dimension ref="A1:D374"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5475,6 +5475,118 @@
         <v>47.65308553728854</v>
       </c>
     </row>
+    <row r="367">
+      <c r="A367" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B367" t="n">
+        <v>0</v>
+      </c>
+      <c r="C367" t="n">
+        <v>2</v>
+      </c>
+      <c r="D367" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="2" t="n">
+        <v>44442</v>
+      </c>
+      <c r="B368" t="n">
+        <v>1</v>
+      </c>
+      <c r="C368" t="n">
+        <v>2</v>
+      </c>
+      <c r="D368" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="2" t="n">
+        <v>44443</v>
+      </c>
+      <c r="B369" t="n">
+        <v>0</v>
+      </c>
+      <c r="C369" t="n">
+        <v>2</v>
+      </c>
+      <c r="D369" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="2" t="n">
+        <v>44444</v>
+      </c>
+      <c r="B370" t="n">
+        <v>0</v>
+      </c>
+      <c r="C370" t="n">
+        <v>2</v>
+      </c>
+      <c r="D370" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="2" t="n">
+        <v>44445</v>
+      </c>
+      <c r="B371" t="n">
+        <v>2</v>
+      </c>
+      <c r="C371" t="n">
+        <v>3</v>
+      </c>
+      <c r="D371" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="2" t="n">
+        <v>44446</v>
+      </c>
+      <c r="B372" t="n">
+        <v>0</v>
+      </c>
+      <c r="C372" t="n">
+        <v>3</v>
+      </c>
+      <c r="D372" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="B373" t="n">
+        <v>0</v>
+      </c>
+      <c r="C373" t="n">
+        <v>3</v>
+      </c>
+      <c r="D373" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B374" t="n">
+        <v>0</v>
+      </c>
+      <c r="C374" t="n">
+        <v>3</v>
+      </c>
+      <c r="D374" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 20/09/2021
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D374"/>
+  <dimension ref="A1:D385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5587,6 +5587,160 @@
         <v>71.47962830593281</v>
       </c>
     </row>
+    <row r="375">
+      <c r="A375" s="2" t="n">
+        <v>44449</v>
+      </c>
+      <c r="B375" t="n">
+        <v>0</v>
+      </c>
+      <c r="C375" t="n">
+        <v>2</v>
+      </c>
+      <c r="D375" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B376" t="n">
+        <v>1</v>
+      </c>
+      <c r="C376" t="n">
+        <v>3</v>
+      </c>
+      <c r="D376" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B377" t="n">
+        <v>0</v>
+      </c>
+      <c r="C377" t="n">
+        <v>3</v>
+      </c>
+      <c r="D377" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B378" t="n">
+        <v>1</v>
+      </c>
+      <c r="C378" t="n">
+        <v>2</v>
+      </c>
+      <c r="D378" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B379" t="n">
+        <v>1</v>
+      </c>
+      <c r="C379" t="n">
+        <v>3</v>
+      </c>
+      <c r="D379" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B380" t="n">
+        <v>0</v>
+      </c>
+      <c r="C380" t="n">
+        <v>3</v>
+      </c>
+      <c r="D380" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="2" t="n">
+        <v>44455</v>
+      </c>
+      <c r="B381" t="n">
+        <v>0</v>
+      </c>
+      <c r="C381" t="n">
+        <v>3</v>
+      </c>
+      <c r="D381" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B382" t="n">
+        <v>0</v>
+      </c>
+      <c r="C382" t="n">
+        <v>3</v>
+      </c>
+      <c r="D382" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="2" t="n">
+        <v>44457</v>
+      </c>
+      <c r="B383" t="n">
+        <v>0</v>
+      </c>
+      <c r="C383" t="n">
+        <v>2</v>
+      </c>
+      <c r="D383" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="2" t="n">
+        <v>44458</v>
+      </c>
+      <c r="B384" t="n">
+        <v>0</v>
+      </c>
+      <c r="C384" t="n">
+        <v>2</v>
+      </c>
+      <c r="D384" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="2" t="n">
+        <v>44459</v>
+      </c>
+      <c r="B385" t="n">
+        <v>0</v>
+      </c>
+      <c r="C385" t="n">
+        <v>1</v>
+      </c>
+      <c r="D385" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento fino a 8/12
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -53,25 +53,92 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -364,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D385"/>
+  <dimension ref="A1:D464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5741,7 +5808,1113 @@
         <v>23.82654276864427</v>
       </c>
     </row>
+    <row r="386">
+      <c r="A386" s="2" t="n">
+        <v>44460</v>
+      </c>
+      <c r="B386" t="n">
+        <v>0</v>
+      </c>
+      <c r="C386" t="n">
+        <v>0</v>
+      </c>
+      <c r="D386" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B387" t="n">
+        <v>0</v>
+      </c>
+      <c r="C387" t="n">
+        <v>0</v>
+      </c>
+      <c r="D387" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="2" t="n">
+        <v>44462</v>
+      </c>
+      <c r="B388" t="n">
+        <v>0</v>
+      </c>
+      <c r="C388" t="n">
+        <v>0</v>
+      </c>
+      <c r="D388" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="2" t="n">
+        <v>44463</v>
+      </c>
+      <c r="B389" t="n">
+        <v>3</v>
+      </c>
+      <c r="C389" t="n">
+        <v>3</v>
+      </c>
+      <c r="D389" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B390" t="n">
+        <v>0</v>
+      </c>
+      <c r="C390" t="n">
+        <v>3</v>
+      </c>
+      <c r="D390" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="2" t="n">
+        <v>44465</v>
+      </c>
+      <c r="B391" t="n">
+        <v>0</v>
+      </c>
+      <c r="C391" t="n">
+        <v>3</v>
+      </c>
+      <c r="D391" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B392" t="n">
+        <v>2</v>
+      </c>
+      <c r="C392" t="n">
+        <v>5</v>
+      </c>
+      <c r="D392" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="2" t="n">
+        <v>44467</v>
+      </c>
+      <c r="B393" t="n">
+        <v>0</v>
+      </c>
+      <c r="C393" t="n">
+        <v>5</v>
+      </c>
+      <c r="D393" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="2" t="n">
+        <v>44468</v>
+      </c>
+      <c r="B394" t="n">
+        <v>0</v>
+      </c>
+      <c r="C394" t="n">
+        <v>5</v>
+      </c>
+      <c r="D394" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B395" t="n">
+        <v>0</v>
+      </c>
+      <c r="C395" t="n">
+        <v>5</v>
+      </c>
+      <c r="D395" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="2" t="n">
+        <v>44470</v>
+      </c>
+      <c r="B396" t="n">
+        <v>0</v>
+      </c>
+      <c r="C396" t="n">
+        <v>2</v>
+      </c>
+      <c r="D396" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="2" t="n">
+        <v>44471</v>
+      </c>
+      <c r="B397" t="n">
+        <v>0</v>
+      </c>
+      <c r="C397" t="n">
+        <v>2</v>
+      </c>
+      <c r="D397" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B398" t="n">
+        <v>0</v>
+      </c>
+      <c r="C398" t="n">
+        <v>2</v>
+      </c>
+      <c r="D398" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B399" t="n">
+        <v>0</v>
+      </c>
+      <c r="C399" t="n">
+        <v>0</v>
+      </c>
+      <c r="D399" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B400" t="n">
+        <v>0</v>
+      </c>
+      <c r="C400" t="n">
+        <v>0</v>
+      </c>
+      <c r="D400" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B401" t="n">
+        <v>1</v>
+      </c>
+      <c r="C401" t="n">
+        <v>1</v>
+      </c>
+      <c r="D401" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B402" t="n">
+        <v>1</v>
+      </c>
+      <c r="C402" t="n">
+        <v>2</v>
+      </c>
+      <c r="D402" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="B403" t="n">
+        <v>0</v>
+      </c>
+      <c r="C403" t="n">
+        <v>2</v>
+      </c>
+      <c r="D403" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B404" t="n">
+        <v>0</v>
+      </c>
+      <c r="C404" t="n">
+        <v>2</v>
+      </c>
+      <c r="D404" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B405" t="n">
+        <v>1</v>
+      </c>
+      <c r="C405" t="n">
+        <v>3</v>
+      </c>
+      <c r="D405" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B406" t="n">
+        <v>1</v>
+      </c>
+      <c r="C406" t="n">
+        <v>4</v>
+      </c>
+      <c r="D406" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="2" t="n">
+        <v>44481</v>
+      </c>
+      <c r="B407" t="n">
+        <v>0</v>
+      </c>
+      <c r="C407" t="n">
+        <v>4</v>
+      </c>
+      <c r="D407" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="2" t="n">
+        <v>44482</v>
+      </c>
+      <c r="B408" t="n">
+        <v>0</v>
+      </c>
+      <c r="C408" t="n">
+        <v>3</v>
+      </c>
+      <c r="D408" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="2" t="n">
+        <v>44483</v>
+      </c>
+      <c r="B409" t="n">
+        <v>0</v>
+      </c>
+      <c r="C409" t="n">
+        <v>2</v>
+      </c>
+      <c r="D409" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="2" t="n">
+        <v>44484</v>
+      </c>
+      <c r="B410" t="n">
+        <v>0</v>
+      </c>
+      <c r="C410" t="n">
+        <v>2</v>
+      </c>
+      <c r="D410" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="2" t="n">
+        <v>44485</v>
+      </c>
+      <c r="B411" t="n">
+        <v>0</v>
+      </c>
+      <c r="C411" t="n">
+        <v>2</v>
+      </c>
+      <c r="D411" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="2" t="n">
+        <v>44486</v>
+      </c>
+      <c r="B412" t="n">
+        <v>0</v>
+      </c>
+      <c r="C412" t="n">
+        <v>1</v>
+      </c>
+      <c r="D412" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B413" t="n">
+        <v>0</v>
+      </c>
+      <c r="C413" t="n">
+        <v>0</v>
+      </c>
+      <c r="D413" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="2" t="n">
+        <v>44488</v>
+      </c>
+      <c r="B414" t="n">
+        <v>0</v>
+      </c>
+      <c r="C414" t="n">
+        <v>0</v>
+      </c>
+      <c r="D414" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="2" t="n">
+        <v>44489</v>
+      </c>
+      <c r="B415" t="n">
+        <v>0</v>
+      </c>
+      <c r="C415" t="n">
+        <v>0</v>
+      </c>
+      <c r="D415" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B416" t="n">
+        <v>0</v>
+      </c>
+      <c r="C416" t="n">
+        <v>0</v>
+      </c>
+      <c r="D416" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B417" t="n">
+        <v>0</v>
+      </c>
+      <c r="C417" t="n">
+        <v>0</v>
+      </c>
+      <c r="D417" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="2" t="n">
+        <v>44492</v>
+      </c>
+      <c r="B418" t="n">
+        <v>0</v>
+      </c>
+      <c r="C418" t="n">
+        <v>0</v>
+      </c>
+      <c r="D418" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="2" t="n">
+        <v>44493</v>
+      </c>
+      <c r="B419" t="n">
+        <v>0</v>
+      </c>
+      <c r="C419" t="n">
+        <v>0</v>
+      </c>
+      <c r="D419" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B420" t="n">
+        <v>0</v>
+      </c>
+      <c r="C420" t="n">
+        <v>0</v>
+      </c>
+      <c r="D420" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="2" t="n">
+        <v>44495</v>
+      </c>
+      <c r="B421" t="n">
+        <v>0</v>
+      </c>
+      <c r="C421" t="n">
+        <v>0</v>
+      </c>
+      <c r="D421" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="2" t="n">
+        <v>44496</v>
+      </c>
+      <c r="B422" t="n">
+        <v>0</v>
+      </c>
+      <c r="C422" t="n">
+        <v>0</v>
+      </c>
+      <c r="D422" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B423" t="n">
+        <v>0</v>
+      </c>
+      <c r="C423" t="n">
+        <v>0</v>
+      </c>
+      <c r="D423" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B424" t="n">
+        <v>0</v>
+      </c>
+      <c r="C424" t="n">
+        <v>0</v>
+      </c>
+      <c r="D424" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B425" t="n">
+        <v>0</v>
+      </c>
+      <c r="C425" t="n">
+        <v>0</v>
+      </c>
+      <c r="D425" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="2" t="n">
+        <v>44500</v>
+      </c>
+      <c r="B426" t="n">
+        <v>0</v>
+      </c>
+      <c r="C426" t="n">
+        <v>0</v>
+      </c>
+      <c r="D426" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="2" t="n">
+        <v>44501</v>
+      </c>
+      <c r="B427" t="n">
+        <v>0</v>
+      </c>
+      <c r="C427" t="n">
+        <v>0</v>
+      </c>
+      <c r="D427" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B428" t="n">
+        <v>0</v>
+      </c>
+      <c r="C428" t="n">
+        <v>0</v>
+      </c>
+      <c r="D428" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="2" t="n">
+        <v>44503</v>
+      </c>
+      <c r="B429" t="n">
+        <v>0</v>
+      </c>
+      <c r="C429" t="n">
+        <v>0</v>
+      </c>
+      <c r="D429" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="2" t="n">
+        <v>44504</v>
+      </c>
+      <c r="B430" t="n">
+        <v>0</v>
+      </c>
+      <c r="C430" t="n">
+        <v>0</v>
+      </c>
+      <c r="D430" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="2" t="n">
+        <v>44505</v>
+      </c>
+      <c r="B431" t="n">
+        <v>1</v>
+      </c>
+      <c r="C431" t="n">
+        <v>1</v>
+      </c>
+      <c r="D431" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="2" t="n">
+        <v>44506</v>
+      </c>
+      <c r="B432" t="n">
+        <v>0</v>
+      </c>
+      <c r="C432" t="n">
+        <v>1</v>
+      </c>
+      <c r="D432" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="2" t="n">
+        <v>44507</v>
+      </c>
+      <c r="B433" t="n">
+        <v>0</v>
+      </c>
+      <c r="C433" t="n">
+        <v>1</v>
+      </c>
+      <c r="D433" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="2" t="n">
+        <v>44508</v>
+      </c>
+      <c r="B434" t="n">
+        <v>0</v>
+      </c>
+      <c r="C434" t="n">
+        <v>1</v>
+      </c>
+      <c r="D434" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="B435" t="n">
+        <v>0</v>
+      </c>
+      <c r="C435" t="n">
+        <v>1</v>
+      </c>
+      <c r="D435" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="2" t="n">
+        <v>44510</v>
+      </c>
+      <c r="B436" t="n">
+        <v>0</v>
+      </c>
+      <c r="C436" t="n">
+        <v>1</v>
+      </c>
+      <c r="D436" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="2" t="n">
+        <v>44511</v>
+      </c>
+      <c r="B437" t="n">
+        <v>0</v>
+      </c>
+      <c r="C437" t="n">
+        <v>1</v>
+      </c>
+      <c r="D437" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="B438" t="n">
+        <v>0</v>
+      </c>
+      <c r="C438" t="n">
+        <v>0</v>
+      </c>
+      <c r="D438" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="2" t="n">
+        <v>44513</v>
+      </c>
+      <c r="B439" t="n">
+        <v>0</v>
+      </c>
+      <c r="C439" t="n">
+        <v>0</v>
+      </c>
+      <c r="D439" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="2" t="n">
+        <v>44514</v>
+      </c>
+      <c r="B440" t="n">
+        <v>0</v>
+      </c>
+      <c r="C440" t="n">
+        <v>0</v>
+      </c>
+      <c r="D440" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B441" t="n">
+        <v>0</v>
+      </c>
+      <c r="C441" t="n">
+        <v>0</v>
+      </c>
+      <c r="D441" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="2" t="n">
+        <v>44516</v>
+      </c>
+      <c r="B442" t="n">
+        <v>1</v>
+      </c>
+      <c r="C442" t="n">
+        <v>1</v>
+      </c>
+      <c r="D442" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B443" t="n">
+        <v>0</v>
+      </c>
+      <c r="C443" t="n">
+        <v>1</v>
+      </c>
+      <c r="D443" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="2" t="n">
+        <v>44518</v>
+      </c>
+      <c r="B444" t="n">
+        <v>0</v>
+      </c>
+      <c r="C444" t="n">
+        <v>1</v>
+      </c>
+      <c r="D444" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="2" t="n">
+        <v>44519</v>
+      </c>
+      <c r="B445" t="n">
+        <v>0</v>
+      </c>
+      <c r="C445" t="n">
+        <v>1</v>
+      </c>
+      <c r="D445" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="2" t="n">
+        <v>44520</v>
+      </c>
+      <c r="B446" t="n">
+        <v>0</v>
+      </c>
+      <c r="C446" t="n">
+        <v>1</v>
+      </c>
+      <c r="D446" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="2" t="n">
+        <v>44521</v>
+      </c>
+      <c r="B447" t="n">
+        <v>0</v>
+      </c>
+      <c r="C447" t="n">
+        <v>1</v>
+      </c>
+      <c r="D447" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="2" t="n">
+        <v>44522</v>
+      </c>
+      <c r="B448" t="n">
+        <v>0</v>
+      </c>
+      <c r="C448" t="n">
+        <v>1</v>
+      </c>
+      <c r="D448" t="n">
+        <v>23.82654276864427</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="2" t="n">
+        <v>44523</v>
+      </c>
+      <c r="B449" t="n">
+        <v>0</v>
+      </c>
+      <c r="C449" t="n">
+        <v>0</v>
+      </c>
+      <c r="D449" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="2" t="n">
+        <v>44524</v>
+      </c>
+      <c r="B450" t="n">
+        <v>4</v>
+      </c>
+      <c r="C450" t="n">
+        <v>4</v>
+      </c>
+      <c r="D450" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="2" t="n">
+        <v>44525</v>
+      </c>
+      <c r="B451" t="n">
+        <v>0</v>
+      </c>
+      <c r="C451" t="n">
+        <v>4</v>
+      </c>
+      <c r="D451" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="2" t="n">
+        <v>44526</v>
+      </c>
+      <c r="B452" t="n">
+        <v>0</v>
+      </c>
+      <c r="C452" t="n">
+        <v>4</v>
+      </c>
+      <c r="D452" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="2" t="n">
+        <v>44527</v>
+      </c>
+      <c r="B453" t="n">
+        <v>0</v>
+      </c>
+      <c r="C453" t="n">
+        <v>4</v>
+      </c>
+      <c r="D453" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="2" t="n">
+        <v>44528</v>
+      </c>
+      <c r="B454" t="n">
+        <v>0</v>
+      </c>
+      <c r="C454" t="n">
+        <v>4</v>
+      </c>
+      <c r="D454" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="2" t="n">
+        <v>44529</v>
+      </c>
+      <c r="B455" t="n">
+        <v>0</v>
+      </c>
+      <c r="C455" t="n">
+        <v>4</v>
+      </c>
+      <c r="D455" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B456" t="n">
+        <v>0</v>
+      </c>
+      <c r="C456" t="n">
+        <v>4</v>
+      </c>
+      <c r="D456" t="n">
+        <v>95.30617107457708</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="2" t="n">
+        <v>44531</v>
+      </c>
+      <c r="B457" t="n">
+        <v>0</v>
+      </c>
+      <c r="C457" t="n">
+        <v>0</v>
+      </c>
+      <c r="D457" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="2" t="n">
+        <v>44532</v>
+      </c>
+      <c r="B458" t="n">
+        <v>2</v>
+      </c>
+      <c r="C458" t="n">
+        <v>2</v>
+      </c>
+      <c r="D458" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="2" t="n">
+        <v>44533</v>
+      </c>
+      <c r="B459" t="n">
+        <v>0</v>
+      </c>
+      <c r="C459" t="n">
+        <v>2</v>
+      </c>
+      <c r="D459" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="2" t="n">
+        <v>44534</v>
+      </c>
+      <c r="B460" t="n">
+        <v>0</v>
+      </c>
+      <c r="C460" t="n">
+        <v>2</v>
+      </c>
+      <c r="D460" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="2" t="n">
+        <v>44535</v>
+      </c>
+      <c r="B461" t="n">
+        <v>0</v>
+      </c>
+      <c r="C461" t="n">
+        <v>2</v>
+      </c>
+      <c r="D461" t="n">
+        <v>47.65308553728854</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B462" t="n">
+        <v>1</v>
+      </c>
+      <c r="C462" t="n">
+        <v>3</v>
+      </c>
+      <c r="D462" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="2" t="n">
+        <v>44537</v>
+      </c>
+      <c r="B463" t="n">
+        <v>2</v>
+      </c>
+      <c r="C463" t="n">
+        <v>5</v>
+      </c>
+      <c r="D463" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="2" t="n">
+        <v>44538</v>
+      </c>
+      <c r="B464" t="n">
+        <v>0</v>
+      </c>
+      <c r="C464" t="n">
+        <v>5</v>
+      </c>
+      <c r="D464" t="n">
+        <v>119.1327138432213</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aggiornamento fino a 6 gennaio 2022
</commit_message>
<xml_diff>
--- a/report_vari/comuni/Bastiglia.xlsx
+++ b/report_vari/comuni/Bastiglia.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D464"/>
+  <dimension ref="A1:D491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6914,6 +6914,384 @@
         <v>119.1327138432213</v>
       </c>
     </row>
+    <row r="465">
+      <c r="A465" s="2" t="n">
+        <v>44539</v>
+      </c>
+      <c r="B465" t="n">
+        <v>0</v>
+      </c>
+      <c r="C465" t="n">
+        <v>3</v>
+      </c>
+      <c r="D465" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="2" t="n">
+        <v>44540</v>
+      </c>
+      <c r="B466" t="n">
+        <v>0</v>
+      </c>
+      <c r="C466" t="n">
+        <v>3</v>
+      </c>
+      <c r="D466" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="2" t="n">
+        <v>44541</v>
+      </c>
+      <c r="B467" t="n">
+        <v>0</v>
+      </c>
+      <c r="C467" t="n">
+        <v>3</v>
+      </c>
+      <c r="D467" t="n">
+        <v>71.47962830593281</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="2" t="n">
+        <v>44542</v>
+      </c>
+      <c r="B468" t="n">
+        <v>4</v>
+      </c>
+      <c r="C468" t="n">
+        <v>7</v>
+      </c>
+      <c r="D468" t="n">
+        <v>166.7857993805099</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="2" t="n">
+        <v>44543</v>
+      </c>
+      <c r="B469" t="n">
+        <v>0</v>
+      </c>
+      <c r="C469" t="n">
+        <v>6</v>
+      </c>
+      <c r="D469" t="n">
+        <v>142.9592566118656</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B470" t="n">
+        <v>2</v>
+      </c>
+      <c r="C470" t="n">
+        <v>6</v>
+      </c>
+      <c r="D470" t="n">
+        <v>142.9592566118656</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="2" t="n">
+        <v>44545</v>
+      </c>
+      <c r="B471" t="n">
+        <v>0</v>
+      </c>
+      <c r="C471" t="n">
+        <v>6</v>
+      </c>
+      <c r="D471" t="n">
+        <v>142.9592566118656</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="2" t="n">
+        <v>44546</v>
+      </c>
+      <c r="B472" t="n">
+        <v>3</v>
+      </c>
+      <c r="C472" t="n">
+        <v>9</v>
+      </c>
+      <c r="D472" t="n">
+        <v>214.4388849177984</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="2" t="n">
+        <v>44547</v>
+      </c>
+      <c r="B473" t="n">
+        <v>0</v>
+      </c>
+      <c r="C473" t="n">
+        <v>9</v>
+      </c>
+      <c r="D473" t="n">
+        <v>214.4388849177984</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="2" t="n">
+        <v>44548</v>
+      </c>
+      <c r="B474" t="n">
+        <v>1</v>
+      </c>
+      <c r="C474" t="n">
+        <v>10</v>
+      </c>
+      <c r="D474" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B475" t="n">
+        <v>2</v>
+      </c>
+      <c r="C475" t="n">
+        <v>8</v>
+      </c>
+      <c r="D475" t="n">
+        <v>190.6123421491542</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="2" t="n">
+        <v>44551</v>
+      </c>
+      <c r="B476" t="n">
+        <v>1</v>
+      </c>
+      <c r="C476" t="n">
+        <v>9</v>
+      </c>
+      <c r="D476" t="n">
+        <v>214.4388849177984</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="2" t="n">
+        <v>44552</v>
+      </c>
+      <c r="B477" t="n">
+        <v>3</v>
+      </c>
+      <c r="C477" t="n">
+        <v>10</v>
+      </c>
+      <c r="D477" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="2" t="n">
+        <v>44553</v>
+      </c>
+      <c r="B478" t="n">
+        <v>0</v>
+      </c>
+      <c r="C478" t="n">
+        <v>10</v>
+      </c>
+      <c r="D478" t="n">
+        <v>238.2654276864427</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="2" t="n">
+        <v>44554</v>
+      </c>
+      <c r="B479" t="n">
+        <v>4</v>
+      </c>
+      <c r="C479" t="n">
+        <v>11</v>
+      </c>
+      <c r="D479" t="n">
+        <v>262.091970455087</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="2" t="n">
+        <v>44555</v>
+      </c>
+      <c r="B480" t="n">
+        <v>4</v>
+      </c>
+      <c r="C480" t="n">
+        <v>15</v>
+      </c>
+      <c r="D480" t="n">
+        <v>357.398141529664</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="2" t="n">
+        <v>44556</v>
+      </c>
+      <c r="B481" t="n">
+        <v>0</v>
+      </c>
+      <c r="C481" t="n">
+        <v>14</v>
+      </c>
+      <c r="D481" t="n">
+        <v>333.5715987610197</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="2" t="n">
+        <v>44557</v>
+      </c>
+      <c r="B482" t="n">
+        <v>5</v>
+      </c>
+      <c r="C482" t="n">
+        <v>17</v>
+      </c>
+      <c r="D482" t="n">
+        <v>405.0512270669526</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="2" t="n">
+        <v>44558</v>
+      </c>
+      <c r="B483" t="n">
+        <v>3</v>
+      </c>
+      <c r="C483" t="n">
+        <v>19</v>
+      </c>
+      <c r="D483" t="n">
+        <v>452.7043126042411</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="2" t="n">
+        <v>44559</v>
+      </c>
+      <c r="B484" t="n">
+        <v>3</v>
+      </c>
+      <c r="C484" t="n">
+        <v>19</v>
+      </c>
+      <c r="D484" t="n">
+        <v>452.7043126042411</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="2" t="n">
+        <v>44560</v>
+      </c>
+      <c r="B485" t="n">
+        <v>4</v>
+      </c>
+      <c r="C485" t="n">
+        <v>23</v>
+      </c>
+      <c r="D485" t="n">
+        <v>548.0104836788182</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="2" t="n">
+        <v>44561</v>
+      </c>
+      <c r="B486" t="n">
+        <v>5</v>
+      </c>
+      <c r="C486" t="n">
+        <v>24</v>
+      </c>
+      <c r="D486" t="n">
+        <v>571.8370264474624</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B487" t="n">
+        <v>13</v>
+      </c>
+      <c r="C487" t="n">
+        <v>33</v>
+      </c>
+      <c r="D487" t="n">
+        <v>786.2759113652609</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="2" t="n">
+        <v>44563</v>
+      </c>
+      <c r="B488" t="n">
+        <v>1</v>
+      </c>
+      <c r="C488" t="n">
+        <v>34</v>
+      </c>
+      <c r="D488" t="n">
+        <v>810.1024541339052</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="2" t="n">
+        <v>44564</v>
+      </c>
+      <c r="B489" t="n">
+        <v>8</v>
+      </c>
+      <c r="C489" t="n">
+        <v>37</v>
+      </c>
+      <c r="D489" t="n">
+        <v>881.582082439838</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="2" t="n">
+        <v>44565</v>
+      </c>
+      <c r="B490" t="n">
+        <v>5</v>
+      </c>
+      <c r="C490" t="n">
+        <v>39</v>
+      </c>
+      <c r="D490" t="n">
+        <v>929.2351679771265</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="B491" t="n">
+        <v>9</v>
+      </c>
+      <c r="C491" t="n">
+        <v>45</v>
+      </c>
+      <c r="D491" t="n">
+        <v>1072.194424588992</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>